<commit_message>
populate db (without major docu)
</commit_message>
<xml_diff>
--- a/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
+++ b/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latticesemiconductor4-my.sharepoint.com/personal/jonathan_bunquin_latticesemi_com/Documents/Documents/GitHub/help_dashboard_django/dashboard/online_help/management/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="362" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD98BB8E-1217-4F1D-AAB5-D064E571716B}"/>
+  <xr:revisionPtr revIDLastSave="505" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73033E83-4EE6-42DD-9117-ED2A9F8AD668}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="284">
   <si>
     <t>Radiant Documentation</t>
   </si>
@@ -1554,6 +1554,15 @@
   </si>
   <si>
     <t>Documentation</t>
+  </si>
+  <si>
+    <t>Adel Jambalos</t>
+  </si>
+  <si>
+    <t>Ave Manriquez</t>
+  </si>
+  <si>
+    <t>Verna Deatras</t>
   </si>
 </sst>
 </file>
@@ -2607,7 +2616,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D232" sqref="D232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -2812,7 +2821,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2835,7 +2844,7 @@
         <v>145</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2963,7 +2972,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -2986,7 +2995,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -3030,7 +3039,7 @@
         <v>14</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -3053,7 +3062,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -3076,7 +3085,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -3120,7 +3129,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -3164,7 +3173,7 @@
         <v>18</v>
       </c>
       <c r="D24" s="108" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E24" s="108" t="s">
         <v>261</v>
@@ -3191,7 +3200,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="108" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E25" s="108" t="s">
         <v>261</v>
@@ -3239,7 +3248,7 @@
         <v>11</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -3262,7 +3271,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -3285,7 +3294,7 @@
         <v>155</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -3308,7 +3317,7 @@
         <v>20</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -3356,7 +3365,7 @@
         <v>11</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -3442,7 +3451,7 @@
         <v>159</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
@@ -3467,7 +3476,7 @@
         <v>160</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="4" t="s">
@@ -3492,7 +3501,7 @@
         <v>11</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
@@ -3515,7 +3524,7 @@
         <v>161</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
@@ -3540,7 +3549,7 @@
         <v>24</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -3563,7 +3572,7 @@
         <v>25</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -3586,7 +3595,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="7"/>
@@ -3609,7 +3618,7 @@
         <v>119</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -3632,7 +3641,7 @@
         <v>27</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -3699,7 +3708,7 @@
         <v>163</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E47" s="28"/>
       <c r="F47" s="28"/>
@@ -3722,7 +3731,7 @@
         <v>164</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E48" s="28"/>
       <c r="F48" s="28"/>
@@ -3745,7 +3754,7 @@
         <v>165</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E49" s="28"/>
       <c r="F49" s="28"/>
@@ -3768,7 +3777,7 @@
         <v>120</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E50" s="28"/>
       <c r="F50" s="28"/>
@@ -3791,7 +3800,7 @@
         <v>166</v>
       </c>
       <c r="D51" s="60" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E51" s="58" t="s">
         <v>262</v>
@@ -3818,7 +3827,7 @@
         <v>166</v>
       </c>
       <c r="D52" s="60" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E52" s="58" t="s">
         <v>262</v>
@@ -3872,7 +3881,7 @@
         <v>29</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -3895,7 +3904,7 @@
         <v>30</v>
       </c>
       <c r="D55" s="81" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E55" s="81" t="s">
         <v>248</v>
@@ -3941,7 +3950,7 @@
         <v>31</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -4006,7 +4015,7 @@
         <v>11</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -4050,7 +4059,7 @@
         <v>34</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="7"/>
@@ -4072,7 +4081,7 @@
         <v>35</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -4095,7 +4104,7 @@
         <v>36</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -4159,7 +4168,7 @@
         <v>203</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E67" s="19"/>
       <c r="F67" s="18"/>
@@ -4203,7 +4212,7 @@
         <v>121</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="18"/>
@@ -4226,7 +4235,7 @@
         <v>122</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="18"/>
@@ -4249,7 +4258,7 @@
         <v>170</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E71" s="18"/>
       <c r="F71" s="18"/>
@@ -4272,7 +4281,7 @@
         <v>133</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="18" t="s">
@@ -4297,7 +4306,7 @@
         <v>133</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="18" t="s">
@@ -4322,7 +4331,7 @@
         <v>125</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
@@ -4603,7 +4612,7 @@
         <v>49</v>
       </c>
       <c r="D87" s="58" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E87" s="58" t="s">
         <v>259</v>
@@ -4931,7 +4940,7 @@
         <v>11</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
@@ -4952,7 +4961,7 @@
         <v>62</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E103" s="6"/>
       <c r="F103" s="4"/>
@@ -4975,7 +4984,7 @@
         <v>11</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -5061,7 +5070,7 @@
         <v>175</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4" t="s">
@@ -5086,7 +5095,7 @@
         <v>64</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
@@ -5151,7 +5160,7 @@
         <v>65</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
@@ -5174,7 +5183,7 @@
         <v>66</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
@@ -5197,7 +5206,7 @@
         <v>67</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -5220,7 +5229,7 @@
         <v>68</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
@@ -5243,7 +5252,7 @@
         <v>69</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -5266,7 +5275,7 @@
         <v>11</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E117" s="4"/>
       <c r="F117" s="4" t="s">
@@ -5291,7 +5300,7 @@
         <v>71</v>
       </c>
       <c r="D118" s="81" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E118" s="81" t="s">
         <v>264</v>
@@ -5318,7 +5327,7 @@
         <v>72</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
@@ -5341,7 +5350,7 @@
         <v>72</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
@@ -5364,7 +5373,7 @@
         <v>72</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
@@ -5387,7 +5396,7 @@
         <v>73</v>
       </c>
       <c r="D122" s="60" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E122" s="58" t="s">
         <v>263</v>
@@ -5433,7 +5442,7 @@
         <v>74</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E124" s="7"/>
       <c r="F124" s="7"/>
@@ -5538,7 +5547,7 @@
         <v>11</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
@@ -5582,7 +5591,7 @@
         <v>80</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E131" s="12"/>
       <c r="F131" s="12"/>
@@ -5605,7 +5614,7 @@
         <v>81</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E132" s="4"/>
       <c r="F132" s="4" t="s">
@@ -5630,7 +5639,7 @@
         <v>279</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
@@ -5653,7 +5662,7 @@
         <v>179</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E134" s="4"/>
       <c r="F134" s="12"/>
@@ -5676,7 +5685,7 @@
         <v>180</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E135" s="4"/>
       <c r="F135" s="4" t="s">
@@ -5701,7 +5710,7 @@
         <v>180</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E136" s="4"/>
       <c r="F136" s="4" t="s">
@@ -5726,7 +5735,7 @@
         <v>82</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
@@ -5749,7 +5758,7 @@
         <v>181</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
@@ -5772,7 +5781,7 @@
         <v>83</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
@@ -5795,7 +5804,7 @@
         <v>182</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
@@ -5839,7 +5848,7 @@
         <v>84</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E142" s="44"/>
       <c r="F142" s="4" t="s">
@@ -5864,7 +5873,7 @@
         <v>85</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E143" s="18"/>
       <c r="F143" s="4"/>
@@ -5887,7 +5896,7 @@
         <v>11</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E144" s="15"/>
       <c r="F144" s="4"/>
@@ -5910,7 +5919,7 @@
         <v>184</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E145" s="12"/>
       <c r="F145" s="12" t="s">
@@ -5935,7 +5944,7 @@
         <v>185</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E146" s="44"/>
       <c r="F146" s="4" t="s">
@@ -5985,7 +5994,7 @@
         <v>11</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E148" s="12"/>
       <c r="F148" s="12"/>
@@ -6006,7 +6015,7 @@
         <v>88</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
@@ -6029,7 +6038,7 @@
         <v>11</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E150" s="6"/>
       <c r="F150" s="6"/>
@@ -6052,7 +6061,7 @@
         <v>187</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E151" s="6"/>
       <c r="F151" s="6"/>
@@ -6098,7 +6107,7 @@
         <v>189</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E153" s="6"/>
       <c r="F153" s="4"/>
@@ -6144,7 +6153,7 @@
         <v>190</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E155" s="6"/>
       <c r="F155" s="4"/>
@@ -6167,7 +6176,7 @@
         <v>190</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E156" s="6"/>
       <c r="F156" s="4"/>
@@ -6213,7 +6222,7 @@
         <v>126</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E158" s="6"/>
       <c r="F158" s="4"/>
@@ -6236,7 +6245,7 @@
         <v>191</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E159" s="6"/>
       <c r="F159" s="4"/>
@@ -6259,7 +6268,7 @@
         <v>192</v>
       </c>
       <c r="D160" s="97" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E160" s="100" t="s">
         <v>256</v>
@@ -6287,7 +6296,7 @@
         <v>131</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E161" s="6"/>
       <c r="F161" s="7" t="s">
@@ -6417,7 +6426,7 @@
         <v>92</v>
       </c>
       <c r="D167" s="81" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E167" s="81" t="s">
         <v>252</v>
@@ -6445,7 +6454,7 @@
         <v>11</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E168" s="4"/>
       <c r="F168" s="4" t="s">
@@ -6470,7 +6479,7 @@
         <v>11</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E169" s="4"/>
       <c r="F169" s="4" t="s">
@@ -6520,7 +6529,7 @@
         <v>11</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E171" s="4"/>
       <c r="F171" s="4" t="s">
@@ -6545,7 +6554,7 @@
         <v>197</v>
       </c>
       <c r="D172" s="81" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E172" s="81" t="s">
         <v>255</v>
@@ -6573,7 +6582,7 @@
         <v>196</v>
       </c>
       <c r="D173" s="88" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E173" s="88" t="s">
         <v>250</v>
@@ -6601,7 +6610,7 @@
         <v>198</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E174" s="4"/>
       <c r="F174" s="4"/>
@@ -6624,7 +6633,7 @@
         <v>198</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E175" s="4"/>
       <c r="F175" s="4"/>
@@ -6670,7 +6679,7 @@
         <v>198</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E177" s="4"/>
       <c r="F177" s="4"/>
@@ -6693,7 +6702,7 @@
         <v>94</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E178" s="4"/>
       <c r="F178" s="4"/>
@@ -6716,7 +6725,7 @@
         <v>94</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E179" s="4"/>
       <c r="F179" s="4"/>
@@ -6762,7 +6771,7 @@
         <v>94</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E181" s="4"/>
       <c r="F181" s="4"/>
@@ -6785,7 +6794,7 @@
         <v>199</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E182" s="4"/>
       <c r="F182" s="4"/>
@@ -6834,7 +6843,7 @@
       </c>
       <c r="C184" s="4"/>
       <c r="D184" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E184" s="4"/>
       <c r="F184" s="4"/>
@@ -6855,7 +6864,7 @@
       </c>
       <c r="C185" s="4"/>
       <c r="D185" s="4" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E185" s="4"/>
       <c r="F185" s="4"/>
@@ -6897,7 +6906,7 @@
       </c>
       <c r="C187" s="4"/>
       <c r="D187" s="4" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E187" s="4"/>
       <c r="F187" s="4"/>
@@ -6918,7 +6927,7 @@
       </c>
       <c r="C188" s="4"/>
       <c r="D188" s="4" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E188" s="4"/>
       <c r="F188" s="4"/>
@@ -6939,7 +6948,7 @@
       </c>
       <c r="C189" s="4"/>
       <c r="D189" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E189" s="4"/>
       <c r="F189" s="4"/>
@@ -6979,7 +6988,7 @@
       </c>
       <c r="C191" s="4"/>
       <c r="D191" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E191" s="4"/>
       <c r="F191" s="4"/>
@@ -7000,7 +7009,7 @@
       </c>
       <c r="C192" s="4"/>
       <c r="D192" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E192" s="4"/>
       <c r="F192" s="4"/>
@@ -7021,7 +7030,7 @@
       </c>
       <c r="C193" s="4"/>
       <c r="D193" s="4" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E193" s="4"/>
       <c r="F193" s="4"/>
@@ -7044,7 +7053,7 @@
         <v>87</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E194" s="6"/>
       <c r="F194" s="4"/>
@@ -7189,7 +7198,7 @@
       </c>
       <c r="C201" s="5"/>
       <c r="D201" s="6" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E201" s="6"/>
       <c r="F201" s="6"/>
@@ -7335,7 +7344,7 @@
         <v>87</v>
       </c>
       <c r="D208" s="76" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E208" s="60" t="s">
         <v>253</v>
@@ -7361,7 +7370,7 @@
         <v>87</v>
       </c>
       <c r="D209" s="76" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E209" s="60" t="s">
         <v>253</v>
@@ -7413,7 +7422,7 @@
         <v>87</v>
       </c>
       <c r="D211" s="76" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E211" s="60" t="s">
         <v>253</v>
@@ -7435,7 +7444,7 @@
       <c r="B212" s="66"/>
       <c r="C212" s="77"/>
       <c r="D212" s="66" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E212" s="66" t="s">
         <v>208</v>
@@ -7457,7 +7466,7 @@
       <c r="B213" s="66"/>
       <c r="C213" s="77"/>
       <c r="D213" s="66" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E213" s="66" t="s">
         <v>208</v>
@@ -7501,7 +7510,7 @@
       <c r="B215" s="66"/>
       <c r="C215" s="77"/>
       <c r="D215" s="66" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E215" s="66" t="s">
         <v>208</v>
@@ -7527,7 +7536,7 @@
         <v>210</v>
       </c>
       <c r="D216" s="12" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E216" s="39" t="s">
         <v>211</v>
@@ -7552,7 +7561,7 @@
         <v>210</v>
       </c>
       <c r="D217" s="12" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E217" s="39" t="s">
         <v>211</v>
@@ -7602,7 +7611,7 @@
         <v>210</v>
       </c>
       <c r="D219" s="12" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E219" s="39" t="s">
         <v>211</v>
@@ -7646,7 +7655,7 @@
       </c>
       <c r="C221" s="5"/>
       <c r="D221" s="4" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E221" s="17"/>
       <c r="F221" s="4"/>
@@ -7688,7 +7697,7 @@
       </c>
       <c r="C223" s="7"/>
       <c r="D223" s="7" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E223" s="4" t="s">
         <v>244</v>
@@ -7711,7 +7720,7 @@
       </c>
       <c r="C224" s="82"/>
       <c r="D224" s="82" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E224" s="81" t="s">
         <v>266</v>
@@ -7758,7 +7767,7 @@
       </c>
       <c r="C226" s="82"/>
       <c r="D226" s="82" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E226" s="81" t="s">
         <v>257</v>
@@ -7782,7 +7791,7 @@
       </c>
       <c r="C227" s="7"/>
       <c r="D227" s="7" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="E227" s="44" t="s">
         <v>260</v>
@@ -7805,7 +7814,7 @@
       </c>
       <c r="C228" s="82"/>
       <c r="D228" s="82" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E228" s="81" t="s">
         <v>265</v>
@@ -7850,7 +7859,7 @@
       </c>
       <c r="C230" s="82"/>
       <c r="D230" s="82" t="s">
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="E230" s="82" t="s">
         <v>267</v>
@@ -7874,7 +7883,7 @@
       </c>
       <c r="C231" s="82"/>
       <c r="D231" s="82" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E231" s="82" t="s">
         <v>267</v>
@@ -7890,6 +7899,7 @@
       <c r="L231" s="84"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L231" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="I71:I73">
     <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I71,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(I71,0)&lt;(WEEKDAY(TODAY())+7))</formula>

</xml_diff>

<commit_message>
98% working ang home_test
color na lang kulang pisti
</commit_message>
<xml_diff>
--- a/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
+++ b/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latticesemiconductor4-my.sharepoint.com/personal/jonathan_bunquin_latticesemi_com/Documents/Documents/GitHub/help_dashboard_django/dashboard/online_help/management/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="505" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73033E83-4EE6-42DD-9117-ED2A9F8AD668}"/>
+  <xr:revisionPtr revIDLastSave="518" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37553857-8AED-4E88-BF7A-868396F10DD9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="ECNs" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025.1'!$A$1:$L$231</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025.1'!$A$1:$M$231</definedName>
     <definedName name="_Hlk95147257" localSheetId="0">'2025.1'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="285">
   <si>
     <t>Radiant Documentation</t>
   </si>
@@ -1563,6 +1563,9 @@
   </si>
   <si>
     <t>Verna Deatras</t>
+  </si>
+  <si>
+    <t>completion</t>
   </si>
 </sst>
 </file>
@@ -1916,7 +1919,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2240,6 +2243,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2612,11 +2618,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L231"/>
+  <dimension ref="A1:M232"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D232" sqref="D232"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P231" sqref="P231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -2634,7 +2640,7 @@
     <col min="11" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="102.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="102.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>280</v>
       </c>
@@ -2668,11 +2674,14 @@
       <c r="K1" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="63" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="63" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="57" t="s">
         <v>8</v>
       </c>
@@ -2696,8 +2705,12 @@
       <c r="K2" s="63" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" s="63" customFormat="1" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L2" s="112" t="str">
+        <f>IF(K2="Yellow", "50%", IF(K2="Green", "100%", IF(K2="Grey", "0%", IF(K2="White", "30%", IF(K2="Orange", "10%", "")))))</f>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="63" customFormat="1" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
@@ -2721,8 +2734,12 @@
       <c r="K3" s="63" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" s="63" customFormat="1" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L3" s="112" t="str">
+        <f t="shared" ref="L3:L66" si="0">IF(K3="Yellow", "50%", IF(K3="Green", "100%", IF(K3="Grey", "0%", IF(K3="White", "30%", IF(K3="Orange", "10%", "")))))</f>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="63" customFormat="1" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="64" t="s">
         <v>8</v>
       </c>
@@ -2746,8 +2763,12 @@
       <c r="K4" s="63" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L4" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -2767,8 +2788,12 @@
       <c r="K5" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L5" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
@@ -2788,8 +2813,12 @@
       <c r="K6" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L6" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2809,8 +2838,12 @@
       <c r="K7" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L7" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -2832,8 +2865,12 @@
       <c r="K8" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L8" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -2855,8 +2892,12 @@
       <c r="K9" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L9" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
@@ -2876,8 +2917,12 @@
       <c r="K10" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L10" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -2897,8 +2942,12 @@
       <c r="K11" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L11" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -2918,8 +2967,12 @@
       <c r="K12" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L12" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
@@ -2939,8 +2992,12 @@
       <c r="K13" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L13" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
@@ -2960,8 +3017,12 @@
       <c r="K14" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="54.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L14" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="54.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>8</v>
       </c>
@@ -2983,8 +3044,12 @@
       <c r="K15" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L15" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
@@ -3006,8 +3071,12 @@
       <c r="K16" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L16" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>8</v>
       </c>
@@ -3027,8 +3096,12 @@
       <c r="K17" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L17" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>8</v>
       </c>
@@ -3050,8 +3123,12 @@
       <c r="K18" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L18" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
@@ -3073,8 +3150,12 @@
       <c r="K19" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L19" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -3096,8 +3177,12 @@
       <c r="K20" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L20" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
@@ -3117,8 +3202,12 @@
       <c r="K21" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L21" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>8</v>
       </c>
@@ -3140,8 +3229,12 @@
       <c r="K22" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L22" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>8</v>
       </c>
@@ -3161,8 +3254,12 @@
       <c r="K23" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L23" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="78" t="s">
         <v>8</v>
       </c>
@@ -3188,8 +3285,12 @@
       <c r="K24" s="84" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L24" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>100%</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="78" t="s">
         <v>8</v>
       </c>
@@ -3215,8 +3316,12 @@
       <c r="K25" s="84" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L25" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>100%</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>8</v>
       </c>
@@ -3236,8 +3341,12 @@
       <c r="K26" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L26" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>8</v>
       </c>
@@ -3259,8 +3368,12 @@
       <c r="K27" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L27" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>8</v>
       </c>
@@ -3282,8 +3395,12 @@
       <c r="K28" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L28" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>8</v>
       </c>
@@ -3305,8 +3422,12 @@
       <c r="K29" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L29" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>8</v>
       </c>
@@ -3328,8 +3449,12 @@
       <c r="K30" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L30" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>8</v>
       </c>
@@ -3353,8 +3478,12 @@
       <c r="K31" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L31" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>8</v>
       </c>
@@ -3376,8 +3505,12 @@
       <c r="K32" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L32" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>8</v>
       </c>
@@ -3397,8 +3530,12 @@
       <c r="K33" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L33" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>8</v>
       </c>
@@ -3418,8 +3555,12 @@
       <c r="K34" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L34" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>8</v>
       </c>
@@ -3439,8 +3580,12 @@
       <c r="K35" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L35" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>8</v>
       </c>
@@ -3464,8 +3609,12 @@
       <c r="K36" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" s="22" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L36" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="22" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
         <v>8</v>
       </c>
@@ -3489,8 +3638,12 @@
       <c r="K37" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L37" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>8</v>
       </c>
@@ -3512,8 +3665,12 @@
       <c r="K38" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L38" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>8</v>
       </c>
@@ -3537,8 +3694,12 @@
       <c r="K39" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L39" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
         <v>8</v>
       </c>
@@ -3560,8 +3721,12 @@
       <c r="K40" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L40" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
         <v>8</v>
       </c>
@@ -3583,8 +3748,12 @@
       <c r="K41" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L41" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>8</v>
       </c>
@@ -3606,8 +3775,12 @@
       <c r="K42" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="26.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L42" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="26.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>8</v>
       </c>
@@ -3629,8 +3802,12 @@
       <c r="K43" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="46.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L43" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="46.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
         <v>8</v>
       </c>
@@ -3652,8 +3829,12 @@
       <c r="K44" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L44" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>8</v>
       </c>
@@ -3673,8 +3854,12 @@
       <c r="K45" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L45" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>8</v>
       </c>
@@ -3696,8 +3881,12 @@
       <c r="K46" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L46" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>8</v>
       </c>
@@ -3719,8 +3908,12 @@
       <c r="K47" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" s="30" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L47" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="30" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>8</v>
       </c>
@@ -3742,8 +3935,12 @@
       <c r="K48" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L48" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>8</v>
       </c>
@@ -3765,8 +3962,12 @@
       <c r="K49" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" s="30" customFormat="1" ht="71.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L49" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="30" customFormat="1" ht="71.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>8</v>
       </c>
@@ -3788,8 +3989,12 @@
       <c r="K50" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L50" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="67" t="s">
         <v>8</v>
       </c>
@@ -3815,8 +4020,12 @@
       <c r="K51" s="72" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L51" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="67" t="s">
         <v>8</v>
       </c>
@@ -3842,8 +4051,12 @@
       <c r="K52" s="72" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L52" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="67" t="s">
         <v>8</v>
       </c>
@@ -3869,8 +4082,12 @@
       <c r="K53" s="72" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L53" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>8</v>
       </c>
@@ -3892,8 +4109,12 @@
       <c r="K54" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" s="84" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L54" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="84" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="78" t="s">
         <v>8</v>
       </c>
@@ -3917,8 +4138,12 @@
       <c r="K55" s="84" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L55" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>100%</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>8</v>
       </c>
@@ -3938,8 +4163,12 @@
       <c r="K56" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L56" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>8</v>
       </c>
@@ -3961,8 +4190,12 @@
       <c r="K57" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L57" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>8</v>
       </c>
@@ -3982,8 +4215,12 @@
       <c r="K58" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L58" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>8</v>
       </c>
@@ -4003,8 +4240,12 @@
       <c r="K59" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L59" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
         <v>8</v>
       </c>
@@ -4026,8 +4267,12 @@
       <c r="K60" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L60" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>8</v>
       </c>
@@ -4047,8 +4292,12 @@
       <c r="K61" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" ht="23.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L61" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="23.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
         <v>8</v>
       </c>
@@ -4069,8 +4318,12 @@
       <c r="K62" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L62" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>8</v>
       </c>
@@ -4092,8 +4345,12 @@
       <c r="K63" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L63" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>8</v>
       </c>
@@ -4115,8 +4372,12 @@
       <c r="K64" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L64" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>8</v>
       </c>
@@ -4135,8 +4396,12 @@
       <c r="K65" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L65" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>8</v>
       </c>
@@ -4156,8 +4421,12 @@
       <c r="K66" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L66" s="112" t="str">
+        <f t="shared" si="0"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>8</v>
       </c>
@@ -4179,8 +4448,12 @@
       <c r="K67" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L67" s="112" t="str">
+        <f t="shared" ref="L67:L130" si="1">IF(K67="Yellow", "50%", IF(K67="Green", "100%", IF(K67="Grey", "0%", IF(K67="White", "30%", IF(K67="Orange", "10%", "")))))</f>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
         <v>8</v>
       </c>
@@ -4200,8 +4473,12 @@
       <c r="K68" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L68" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>8</v>
       </c>
@@ -4223,8 +4500,12 @@
       <c r="K69" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L69" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>8</v>
       </c>
@@ -4246,8 +4527,12 @@
       <c r="K70" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L70" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
         <v>8</v>
       </c>
@@ -4269,8 +4554,12 @@
       <c r="K71" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L71" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>8</v>
       </c>
@@ -4294,8 +4583,12 @@
       <c r="K72" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L72" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>8</v>
       </c>
@@ -4319,8 +4612,12 @@
       <c r="K73" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L73" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>8</v>
       </c>
@@ -4342,8 +4639,12 @@
       <c r="K74" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L74" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>8</v>
       </c>
@@ -4363,8 +4664,12 @@
       <c r="K75" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L75" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
         <v>8</v>
       </c>
@@ -4384,8 +4689,12 @@
       <c r="K76" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L76" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
         <v>8</v>
       </c>
@@ -4405,8 +4714,12 @@
       <c r="K77" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L77" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="s">
         <v>8</v>
       </c>
@@ -4426,8 +4739,12 @@
       <c r="K78" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L78" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
         <v>8</v>
       </c>
@@ -4447,8 +4764,12 @@
       <c r="K79" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L79" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="s">
         <v>8</v>
       </c>
@@ -4468,8 +4789,12 @@
       <c r="K80" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L80" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A81" s="10" t="s">
         <v>8</v>
       </c>
@@ -4489,8 +4814,12 @@
       <c r="K81" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L81" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="10" t="s">
         <v>8</v>
       </c>
@@ -4510,8 +4839,12 @@
       <c r="K82" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L82" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A83" s="10" t="s">
         <v>8</v>
       </c>
@@ -4531,8 +4864,12 @@
       <c r="K83" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L83" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A84" s="10" t="s">
         <v>8</v>
       </c>
@@ -4552,8 +4889,12 @@
       <c r="K84" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" s="63" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L84" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" s="63" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="64" t="s">
         <v>8</v>
       </c>
@@ -4579,8 +4920,12 @@
       <c r="K85" s="63" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L85" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="10" t="s">
         <v>8</v>
       </c>
@@ -4600,8 +4945,12 @@
       <c r="K86" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" s="63" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L86" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" s="63" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="s">
         <v>8</v>
       </c>
@@ -4627,8 +4976,12 @@
       <c r="K87" s="63" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" s="63" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L87" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" s="63" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="s">
         <v>8</v>
       </c>
@@ -4654,8 +5007,12 @@
       <c r="K88" s="63" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L88" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="10" t="s">
         <v>8</v>
       </c>
@@ -4675,8 +5032,12 @@
       <c r="K89" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L89" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A90" s="10" t="s">
         <v>8</v>
       </c>
@@ -4696,8 +5057,12 @@
       <c r="K90" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L90" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="10" t="s">
         <v>8</v>
       </c>
@@ -4717,8 +5082,12 @@
       <c r="K91" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L91" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="10" t="s">
         <v>8</v>
       </c>
@@ -4738,8 +5107,12 @@
       <c r="K92" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L92" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="10" t="s">
         <v>8</v>
       </c>
@@ -4759,8 +5132,12 @@
       <c r="K93" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L93" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A94" s="10" t="s">
         <v>8</v>
       </c>
@@ -4780,8 +5157,12 @@
       <c r="K94" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L94" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A95" s="10" t="s">
         <v>8</v>
       </c>
@@ -4801,8 +5182,12 @@
       <c r="K95" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L95" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="10" t="s">
         <v>8</v>
       </c>
@@ -4822,8 +5207,12 @@
       <c r="K96" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L96" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
         <v>8</v>
       </c>
@@ -4845,8 +5234,12 @@
       <c r="K97" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L97" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
         <v>8</v>
       </c>
@@ -4866,8 +5259,12 @@
       <c r="K98" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L98" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10" t="s">
         <v>8</v>
       </c>
@@ -4887,8 +5284,12 @@
       <c r="K99" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L99" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="10" t="s">
         <v>8</v>
       </c>
@@ -4908,8 +5309,12 @@
       <c r="K100" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L100" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="s">
         <v>8</v>
       </c>
@@ -4928,8 +5333,12 @@
       <c r="K101" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L101" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A102" s="10" t="s">
         <v>8</v>
       </c>
@@ -4951,8 +5360,12 @@
       <c r="K102" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L102" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A103" s="10" t="s">
         <v>8</v>
       </c>
@@ -4972,8 +5385,12 @@
       <c r="K103" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L103" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="10" t="s">
         <v>8</v>
       </c>
@@ -4995,8 +5412,12 @@
       <c r="K104" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L104" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10" t="s">
         <v>8</v>
       </c>
@@ -5016,8 +5437,12 @@
       <c r="K105" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L105" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="10" t="s">
         <v>8</v>
       </c>
@@ -5037,8 +5462,12 @@
       <c r="K106" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L106" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="s">
         <v>8</v>
       </c>
@@ -5058,8 +5487,12 @@
       <c r="K107" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L107" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A108" s="10" t="s">
         <v>8</v>
       </c>
@@ -5083,8 +5516,12 @@
       <c r="K108" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L108" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
         <v>8</v>
       </c>
@@ -5106,8 +5543,12 @@
       <c r="K109" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L109" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A110" s="10" t="s">
         <v>8</v>
       </c>
@@ -5127,8 +5568,12 @@
       <c r="K110" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="L110" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A111" s="10" t="s">
         <v>8</v>
       </c>
@@ -5148,8 +5593,12 @@
       <c r="K111" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L111" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A112" s="10" t="s">
         <v>8</v>
       </c>
@@ -5171,8 +5620,12 @@
       <c r="K112" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L112" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A113" s="10" t="s">
         <v>8</v>
       </c>
@@ -5194,8 +5647,12 @@
       <c r="K113" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L113" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="s">
         <v>8</v>
       </c>
@@ -5217,8 +5674,12 @@
       <c r="K114" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L114" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="s">
         <v>8</v>
       </c>
@@ -5240,8 +5701,12 @@
       <c r="K115" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L115" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="10" t="s">
         <v>8</v>
       </c>
@@ -5263,8 +5728,12 @@
       <c r="K116" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L116" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="10" t="s">
         <v>8</v>
       </c>
@@ -5288,8 +5757,12 @@
       <c r="K117" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" s="84" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L117" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" s="84" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="78" t="s">
         <v>8</v>
       </c>
@@ -5315,8 +5788,12 @@
       <c r="K118" s="84" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L118" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>100%</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="10" t="s">
         <v>8</v>
       </c>
@@ -5338,8 +5815,12 @@
       <c r="K119" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L119" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="10" t="s">
         <v>8</v>
       </c>
@@ -5361,8 +5842,12 @@
       <c r="K120" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L120" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="10" t="s">
         <v>8</v>
       </c>
@@ -5384,8 +5869,12 @@
       <c r="K121" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" s="63" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L121" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" s="63" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="64" t="s">
         <v>8</v>
       </c>
@@ -5411,8 +5900,12 @@
       <c r="K122" s="63" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" ht="31.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L122" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>50%</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="31.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="19" t="s">
         <v>8</v>
       </c>
@@ -5430,8 +5923,12 @@
       <c r="K123" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L123" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A124" s="19" t="s">
         <v>8</v>
       </c>
@@ -5451,8 +5948,12 @@
       <c r="K124" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L124" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A125" s="19" t="s">
         <v>8</v>
       </c>
@@ -5472,8 +5973,12 @@
       <c r="K125" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L125" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A126" s="19" t="s">
         <v>8</v>
       </c>
@@ -5493,8 +5998,12 @@
       <c r="K126" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L126" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A127" s="19" t="s">
         <v>8</v>
       </c>
@@ -5514,8 +6023,12 @@
       <c r="K127" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L127" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A128" s="19" t="s">
         <v>8</v>
       </c>
@@ -5535,8 +6048,12 @@
       <c r="K128" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L128" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A129" s="10" t="s">
         <v>78</v>
       </c>
@@ -5558,8 +6075,12 @@
       <c r="K129" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L129" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A130" s="10" t="s">
         <v>78</v>
       </c>
@@ -5579,8 +6100,12 @@
       <c r="K130" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L130" s="112" t="str">
+        <f t="shared" si="1"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A131" s="10" t="s">
         <v>78</v>
       </c>
@@ -5602,8 +6127,12 @@
       <c r="K131" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L131" s="112" t="str">
+        <f t="shared" ref="L131:L194" si="2">IF(K131="Yellow", "50%", IF(K131="Green", "100%", IF(K131="Grey", "0%", IF(K131="White", "30%", IF(K131="Orange", "10%", "")))))</f>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A132" s="10" t="s">
         <v>78</v>
       </c>
@@ -5627,8 +6156,12 @@
       <c r="K132" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L132" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A133" s="10" t="s">
         <v>78</v>
       </c>
@@ -5650,8 +6183,12 @@
       <c r="K133" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L133" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A134" s="10" t="s">
         <v>78</v>
       </c>
@@ -5673,8 +6210,12 @@
       <c r="K134" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L134" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A135" s="10" t="s">
         <v>78</v>
       </c>
@@ -5698,8 +6239,12 @@
       <c r="K135" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L135" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A136" s="10" t="s">
         <v>78</v>
       </c>
@@ -5723,8 +6268,12 @@
       <c r="K136" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L136" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A137" s="10" t="s">
         <v>78</v>
       </c>
@@ -5746,8 +6295,12 @@
       <c r="K137" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L137" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A138" s="10" t="s">
         <v>78</v>
       </c>
@@ -5769,8 +6322,12 @@
       <c r="K138" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L138" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A139" s="10" t="s">
         <v>78</v>
       </c>
@@ -5792,8 +6349,12 @@
       <c r="K139" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L139" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A140" s="10" t="s">
         <v>78</v>
       </c>
@@ -5815,8 +6376,12 @@
       <c r="K140" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L140" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A141" s="10" t="s">
         <v>78</v>
       </c>
@@ -5836,8 +6401,12 @@
       <c r="K141" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L141" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A142" s="10" t="s">
         <v>78</v>
       </c>
@@ -5861,8 +6430,12 @@
       <c r="K142" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L142" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A143" s="10" t="s">
         <v>78</v>
       </c>
@@ -5884,8 +6457,12 @@
       <c r="K143" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="L143" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A144" s="10" t="s">
         <v>78</v>
       </c>
@@ -5907,8 +6484,12 @@
       <c r="K144" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L144" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A145" s="10" t="s">
         <v>78</v>
       </c>
@@ -5932,8 +6513,12 @@
       <c r="K145" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L145" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A146" s="10" t="s">
         <v>78</v>
       </c>
@@ -5957,8 +6542,12 @@
       <c r="K146" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L146" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A147" s="10" t="s">
         <v>78</v>
       </c>
@@ -5982,8 +6571,12 @@
       <c r="K147" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L147" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A148" s="10" t="s">
         <v>78</v>
       </c>
@@ -6005,8 +6598,12 @@
       <c r="K148" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L148" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A149" s="10" t="s">
         <v>78</v>
       </c>
@@ -6026,8 +6623,12 @@
       <c r="K149" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L149" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A150" s="10" t="s">
         <v>78</v>
       </c>
@@ -6049,8 +6650,12 @@
       <c r="K150" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L150" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A151" s="10" t="s">
         <v>78</v>
       </c>
@@ -6072,8 +6677,12 @@
       <c r="K151" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L151" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A152" s="10" t="s">
         <v>78</v>
       </c>
@@ -6095,8 +6704,12 @@
       <c r="K152" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="L152" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A153" s="10" t="s">
         <v>78</v>
       </c>
@@ -6118,8 +6731,12 @@
       <c r="K153" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L153" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A154" s="10" t="s">
         <v>78</v>
       </c>
@@ -6141,8 +6758,12 @@
       <c r="K154" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L154" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A155" s="10" t="s">
         <v>78</v>
       </c>
@@ -6164,8 +6785,12 @@
       <c r="K155" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L155" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A156" s="10" t="s">
         <v>78</v>
       </c>
@@ -6187,8 +6812,12 @@
       <c r="K156" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L156" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A157" s="10" t="s">
         <v>78</v>
       </c>
@@ -6210,8 +6839,12 @@
       <c r="K157" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L157" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A158" s="10" t="s">
         <v>78</v>
       </c>
@@ -6233,8 +6866,12 @@
       <c r="K158" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L158" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A159" s="10" t="s">
         <v>78</v>
       </c>
@@ -6256,8 +6893,12 @@
       <c r="K159" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L159" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A160" s="85" t="s">
         <v>78</v>
       </c>
@@ -6283,9 +6924,13 @@
       <c r="K160" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="L160" s="93"/>
-    </row>
-    <row r="161" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L160" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>10%</v>
+      </c>
+      <c r="M160" s="93"/>
+    </row>
+    <row r="161" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A161" s="10" t="s">
         <v>78</v>
       </c>
@@ -6309,8 +6954,12 @@
       <c r="K161" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="162" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L161" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A162" s="10" t="s">
         <v>78</v>
       </c>
@@ -6330,8 +6979,12 @@
       <c r="K162" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L162" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A163" s="10" t="s">
         <v>78</v>
       </c>
@@ -6351,8 +7004,12 @@
       <c r="K163" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="164" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L163" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A164" s="10" t="s">
         <v>78</v>
       </c>
@@ -6372,8 +7029,12 @@
       <c r="K164" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="165" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L164" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A165" s="10" t="s">
         <v>78</v>
       </c>
@@ -6393,8 +7054,12 @@
       <c r="K165" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="166" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L165" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A166" s="10" t="s">
         <v>78</v>
       </c>
@@ -6414,8 +7079,12 @@
       <c r="K166" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="167" spans="1:12" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="L166" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A167" s="78" t="s">
         <v>78</v>
       </c>
@@ -6441,9 +7110,13 @@
       <c r="K167" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L167" s="84"/>
-    </row>
-    <row r="168" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L167" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>100%</v>
+      </c>
+      <c r="M167" s="84"/>
+    </row>
+    <row r="168" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A168" s="10" t="s">
         <v>78</v>
       </c>
@@ -6467,8 +7140,12 @@
       <c r="K168" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="169" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L168" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A169" s="10" t="s">
         <v>78</v>
       </c>
@@ -6492,8 +7169,12 @@
       <c r="K169" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="170" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L169" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A170" s="10" t="s">
         <v>78</v>
       </c>
@@ -6517,8 +7198,12 @@
       <c r="K170" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="171" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L170" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A171" s="10" t="s">
         <v>78</v>
       </c>
@@ -6542,8 +7227,12 @@
       <c r="K171" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="172" spans="1:12" ht="38.5" x14ac:dyDescent="0.3">
+      <c r="L171" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A172" s="78" t="s">
         <v>78</v>
       </c>
@@ -6569,9 +7258,13 @@
       <c r="K172" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L172" s="84"/>
-    </row>
-    <row r="173" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="L172" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>100%</v>
+      </c>
+      <c r="M172" s="84"/>
+    </row>
+    <row r="173" spans="1:13" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A173" s="85" t="s">
         <v>78</v>
       </c>
@@ -6597,9 +7290,13 @@
       <c r="K173" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="L173" s="93"/>
-    </row>
-    <row r="174" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="L173" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>10%</v>
+      </c>
+      <c r="M173" s="93"/>
+    </row>
+    <row r="174" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A174" s="10" t="s">
         <v>78</v>
       </c>
@@ -6621,8 +7318,12 @@
       <c r="K174" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="175" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="L174" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A175" s="10" t="s">
         <v>78</v>
       </c>
@@ -6644,8 +7345,12 @@
       <c r="K175" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="176" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="L175" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="s">
         <v>78</v>
       </c>
@@ -6667,8 +7372,12 @@
       <c r="K176" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="L176" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A177" s="10" t="s">
         <v>78</v>
       </c>
@@ -6690,8 +7399,12 @@
       <c r="K177" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="178" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L177" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A178" s="10" t="s">
         <v>78</v>
       </c>
@@ -6713,8 +7426,12 @@
       <c r="K178" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L178" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A179" s="10" t="s">
         <v>78</v>
       </c>
@@ -6736,8 +7453,12 @@
       <c r="K179" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L179" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A180" s="10" t="s">
         <v>78</v>
       </c>
@@ -6759,8 +7480,12 @@
       <c r="K180" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="181" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L180" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A181" s="10" t="s">
         <v>78</v>
       </c>
@@ -6782,8 +7507,12 @@
       <c r="K181" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L181" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A182" s="10" t="s">
         <v>78</v>
       </c>
@@ -6805,8 +7534,12 @@
       <c r="K182" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="183" spans="1:12" ht="64.5" x14ac:dyDescent="0.35">
+      <c r="L182" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" ht="64.5" x14ac:dyDescent="0.35">
       <c r="A183" s="64" t="s">
         <v>78</v>
       </c>
@@ -6832,9 +7565,13 @@
       <c r="K183" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L183" s="63"/>
-    </row>
-    <row r="184" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L183" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>50%</v>
+      </c>
+      <c r="M183" s="63"/>
+    </row>
+    <row r="184" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A184" s="10" t="s">
         <v>95</v>
       </c>
@@ -6854,8 +7591,12 @@
       <c r="K184" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L184" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A185" s="10" t="s">
         <v>95</v>
       </c>
@@ -6875,8 +7616,12 @@
       <c r="K185" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="186" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L185" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A186" s="10" t="s">
         <v>95</v>
       </c>
@@ -6896,8 +7641,12 @@
       <c r="K186" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="187" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L186" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A187" s="10" t="s">
         <v>95</v>
       </c>
@@ -6917,8 +7666,12 @@
       <c r="K187" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L187" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A188" s="10" t="s">
         <v>95</v>
       </c>
@@ -6938,8 +7691,12 @@
       <c r="K188" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="189" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L188" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A189" s="10" t="s">
         <v>95</v>
       </c>
@@ -6959,8 +7716,12 @@
       <c r="K189" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="190" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L189" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A190" s="10" t="s">
         <v>95</v>
       </c>
@@ -6978,8 +7739,12 @@
       <c r="K190" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="191" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L190" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A191" s="10" t="s">
         <v>95</v>
       </c>
@@ -6999,8 +7764,12 @@
       <c r="K191" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="192" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L191" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A192" s="10" t="s">
         <v>100</v>
       </c>
@@ -7020,8 +7789,12 @@
       <c r="K192" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L192" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A193" s="10" t="s">
         <v>100</v>
       </c>
@@ -7041,8 +7814,12 @@
       <c r="K193" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L193" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A194" s="10" t="s">
         <v>100</v>
       </c>
@@ -7064,8 +7841,12 @@
       <c r="K194" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L194" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A195" s="10" t="s">
         <v>100</v>
       </c>
@@ -7085,8 +7866,12 @@
       <c r="K195" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="196" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L195" s="112" t="str">
+        <f t="shared" ref="L195:L232" si="3">IF(K195="Yellow", "50%", IF(K195="Green", "100%", IF(K195="Grey", "0%", IF(K195="White", "30%", IF(K195="Orange", "10%", "")))))</f>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A196" s="10" t="s">
         <v>100</v>
       </c>
@@ -7106,8 +7891,12 @@
       <c r="K196" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="197" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L196" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A197" s="10" t="s">
         <v>100</v>
       </c>
@@ -7127,8 +7916,12 @@
       <c r="K197" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L197" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A198" s="10" t="s">
         <v>100</v>
       </c>
@@ -7146,8 +7939,12 @@
       <c r="K198" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="199" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L198" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A199" s="10" t="s">
         <v>100</v>
       </c>
@@ -7167,8 +7964,12 @@
       <c r="K199" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="200" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L199" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A200" s="10" t="s">
         <v>100</v>
       </c>
@@ -7188,8 +7989,12 @@
       <c r="K200" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L200" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A201" s="10" t="s">
         <v>100</v>
       </c>
@@ -7209,8 +8014,12 @@
       <c r="K201" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="202" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L201" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A202" s="10" t="s">
         <v>100</v>
       </c>
@@ -7230,8 +8039,12 @@
       <c r="K202" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L202" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A203" s="10" t="s">
         <v>100</v>
       </c>
@@ -7253,9 +8066,13 @@
       <c r="K203" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L203" s="45"/>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L203" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+      <c r="M203" s="45"/>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A204" s="10" t="s">
         <v>100</v>
       </c>
@@ -7273,8 +8090,12 @@
       <c r="K204" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L204" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A205" s="10" t="s">
         <v>100</v>
       </c>
@@ -7292,8 +8113,12 @@
       <c r="K205" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L205" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A206" s="10" t="s">
         <v>100</v>
       </c>
@@ -7311,8 +8136,12 @@
       <c r="K206" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L206" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A207" s="10" t="s">
         <v>100</v>
       </c>
@@ -7332,8 +8161,12 @@
       <c r="K207" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="L207" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A208" s="64" t="s">
         <v>100</v>
       </c>
@@ -7357,9 +8190,13 @@
       <c r="K208" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L208" s="63"/>
-    </row>
-    <row r="209" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="L208" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>50%</v>
+      </c>
+      <c r="M208" s="63"/>
+    </row>
+    <row r="209" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A209" s="64" t="s">
         <v>100</v>
       </c>
@@ -7383,9 +8220,13 @@
       <c r="K209" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L209" s="63"/>
-    </row>
-    <row r="210" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="L209" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>50%</v>
+      </c>
+      <c r="M209" s="63"/>
+    </row>
+    <row r="210" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A210" s="64" t="s">
         <v>100</v>
       </c>
@@ -7409,9 +8250,13 @@
       <c r="K210" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L210" s="63"/>
-    </row>
-    <row r="211" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="L210" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>50%</v>
+      </c>
+      <c r="M210" s="63"/>
+    </row>
+    <row r="211" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A211" s="64" t="s">
         <v>100</v>
       </c>
@@ -7435,9 +8280,13 @@
       <c r="K211" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L211" s="63"/>
-    </row>
-    <row r="212" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="L211" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>50%</v>
+      </c>
+      <c r="M211" s="63"/>
+    </row>
+    <row r="212" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A212" s="64" t="s">
         <v>100</v>
       </c>
@@ -7457,9 +8306,13 @@
       <c r="K212" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L212" s="63"/>
-    </row>
-    <row r="213" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="L212" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>50%</v>
+      </c>
+      <c r="M212" s="63"/>
+    </row>
+    <row r="213" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A213" s="64" t="s">
         <v>100</v>
       </c>
@@ -7479,9 +8332,13 @@
       <c r="K213" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L213" s="63"/>
-    </row>
-    <row r="214" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="L213" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>50%</v>
+      </c>
+      <c r="M213" s="63"/>
+    </row>
+    <row r="214" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A214" s="64" t="s">
         <v>100</v>
       </c>
@@ -7501,9 +8358,13 @@
       <c r="K214" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L214" s="63"/>
-    </row>
-    <row r="215" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="L214" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>50%</v>
+      </c>
+      <c r="M214" s="63"/>
+    </row>
+    <row r="215" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A215" s="64" t="s">
         <v>100</v>
       </c>
@@ -7523,9 +8384,13 @@
       <c r="K215" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L215" s="63"/>
-    </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L215" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>50%</v>
+      </c>
+      <c r="M215" s="63"/>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A216" s="10" t="s">
         <v>100</v>
       </c>
@@ -7549,8 +8414,12 @@
       <c r="K216" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L216" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A217" s="10" t="s">
         <v>100</v>
       </c>
@@ -7574,8 +8443,12 @@
       <c r="K217" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="218" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L217" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A218" s="10" t="s">
         <v>100</v>
       </c>
@@ -7599,8 +8472,12 @@
       <c r="K218" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L218" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A219" s="10" t="s">
         <v>100</v>
       </c>
@@ -7624,8 +8501,12 @@
       <c r="K219" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="220" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+      <c r="L219" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A220" s="10" t="s">
         <v>100</v>
       </c>
@@ -7645,8 +8526,12 @@
       <c r="K220" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="221" spans="1:12" ht="13" x14ac:dyDescent="0.35">
+      <c r="L220" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" ht="13" x14ac:dyDescent="0.35">
       <c r="A221" s="10" t="s">
         <v>100</v>
       </c>
@@ -7666,8 +8551,12 @@
       <c r="K221" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="222" spans="1:12" ht="13" x14ac:dyDescent="0.35">
+      <c r="L221" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" ht="13" x14ac:dyDescent="0.35">
       <c r="A222" s="10" t="s">
         <v>100</v>
       </c>
@@ -7687,8 +8576,12 @@
       <c r="K222" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L222" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A223" s="10" t="s">
         <v>100</v>
       </c>
@@ -7710,8 +8603,12 @@
       <c r="K223" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="224" spans="1:12" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="L223" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A224" s="84" t="s">
         <v>100</v>
       </c>
@@ -7733,9 +8630,13 @@
       <c r="K224" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L224" s="84"/>
-    </row>
-    <row r="225" spans="1:12" ht="39" x14ac:dyDescent="0.35">
+      <c r="L224" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>100%</v>
+      </c>
+      <c r="M224" s="84"/>
+    </row>
+    <row r="225" spans="1:13" ht="39" x14ac:dyDescent="0.35">
       <c r="A225" s="9" t="s">
         <v>100</v>
       </c>
@@ -7757,8 +8658,12 @@
       <c r="K225" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="226" spans="1:12" ht="51.5" x14ac:dyDescent="0.35">
+      <c r="L225" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" ht="51.5" x14ac:dyDescent="0.35">
       <c r="A226" s="84" t="s">
         <v>100</v>
       </c>
@@ -7780,9 +8685,13 @@
       <c r="K226" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L226" s="84"/>
-    </row>
-    <row r="227" spans="1:12" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="L226" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>100%</v>
+      </c>
+      <c r="M226" s="84"/>
+    </row>
+    <row r="227" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A227" s="9" t="s">
         <v>100</v>
       </c>
@@ -7804,8 +8713,12 @@
       <c r="K227" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="228" spans="1:12" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="L227" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A228" s="84" t="s">
         <v>100</v>
       </c>
@@ -7827,9 +8740,13 @@
       <c r="K228" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L228" s="84"/>
-    </row>
-    <row r="229" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="L228" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>100%</v>
+      </c>
+      <c r="M228" s="84"/>
+    </row>
+    <row r="229" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A229" s="9" t="s">
         <v>100</v>
       </c>
@@ -7849,8 +8766,12 @@
       <c r="K229" s="9" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="230" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="L229" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A230" s="84" t="s">
         <v>100</v>
       </c>
@@ -7872,9 +8793,13 @@
       <c r="K230" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L230" s="84"/>
-    </row>
-    <row r="231" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="L230" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>100%</v>
+      </c>
+      <c r="M230" s="84"/>
+    </row>
+    <row r="231" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A231" s="84" t="s">
         <v>100</v>
       </c>
@@ -7896,10 +8821,17 @@
       <c r="K231" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L231" s="84"/>
+      <c r="L231" s="112" t="str">
+        <f t="shared" si="3"/>
+        <v>100%</v>
+      </c>
+      <c r="M231" s="84"/>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="L232" s="112"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L231" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M231" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="I71:I73">
     <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I71,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(I71,0)&lt;(WEEKDAY(TODAY())+7))</formula>

</xml_diff>

<commit_message>
editable test semi goods
yung edit per section na lang na makakabawas at dagdag ng subsection, wala pa
</commit_message>
<xml_diff>
--- a/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
+++ b/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latticesemiconductor4-my.sharepoint.com/personal/jonathan_bunquin_latticesemi_com/Documents/Documents/GitHub/help_dashboard_django/dashboard/online_help/management/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="518" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37553857-8AED-4E88-BF7A-868396F10DD9}"/>
+  <xr:revisionPtr revIDLastSave="519" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B07D848E-BB74-42F2-81C5-FA17617C2EB3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1919,7 +1919,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2243,9 +2243,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2618,11 +2615,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M232"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:M231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P231" sqref="P231"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -2705,7 +2703,7 @@
       <c r="K2" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L2" s="112" t="str">
+      <c r="L2" s="9" t="str">
         <f>IF(K2="Yellow", "50%", IF(K2="Green", "100%", IF(K2="Grey", "0%", IF(K2="White", "30%", IF(K2="Orange", "10%", "")))))</f>
         <v>50%</v>
       </c>
@@ -2734,7 +2732,7 @@
       <c r="K3" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L3" s="112" t="str">
+      <c r="L3" s="9" t="str">
         <f t="shared" ref="L3:L66" si="0">IF(K3="Yellow", "50%", IF(K3="Green", "100%", IF(K3="Grey", "0%", IF(K3="White", "30%", IF(K3="Orange", "10%", "")))))</f>
         <v>50%</v>
       </c>
@@ -2763,7 +2761,7 @@
       <c r="K4" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L4" s="112" t="str">
+      <c r="L4" s="9" t="str">
         <f t="shared" si="0"/>
         <v>50%</v>
       </c>
@@ -2788,7 +2786,7 @@
       <c r="K5" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L5" s="112" t="str">
+      <c r="L5" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
@@ -2813,7 +2811,7 @@
       <c r="K6" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L6" s="112" t="str">
+      <c r="L6" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
@@ -2838,12 +2836,12 @@
       <c r="K7" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L7" s="112" t="str">
+      <c r="L7" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -2865,12 +2863,12 @@
       <c r="K8" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L8" s="112" t="str">
+      <c r="L8" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -2892,12 +2890,12 @@
       <c r="K9" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L9" s="112" t="str">
+      <c r="L9" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
@@ -2917,12 +2915,12 @@
       <c r="K10" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L10" s="112" t="str">
+      <c r="L10" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -2942,12 +2940,12 @@
       <c r="K11" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L11" s="112" t="str">
+      <c r="L11" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -2967,12 +2965,12 @@
       <c r="K12" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L12" s="112" t="str">
+      <c r="L12" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
@@ -2992,12 +2990,12 @@
       <c r="K13" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L13" s="112" t="str">
+      <c r="L13" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
@@ -3017,12 +3015,12 @@
       <c r="K14" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L14" s="112" t="str">
+      <c r="L14" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="54.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="54.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>8</v>
       </c>
@@ -3044,12 +3042,12 @@
       <c r="K15" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L15" s="112" t="str">
+      <c r="L15" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
@@ -3071,12 +3069,12 @@
       <c r="K16" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L16" s="112" t="str">
+      <c r="L16" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>8</v>
       </c>
@@ -3096,12 +3094,12 @@
       <c r="K17" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L17" s="112" t="str">
+      <c r="L17" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>8</v>
       </c>
@@ -3123,12 +3121,12 @@
       <c r="K18" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L18" s="112" t="str">
+      <c r="L18" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="65.150000000000006" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
@@ -3150,12 +3148,12 @@
       <c r="K19" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L19" s="112" t="str">
+      <c r="L19" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="15.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -3177,12 +3175,12 @@
       <c r="K20" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L20" s="112" t="str">
+      <c r="L20" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="15.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
@@ -3202,12 +3200,12 @@
       <c r="K21" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L21" s="112" t="str">
+      <c r="L21" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="35.15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>8</v>
       </c>
@@ -3229,12 +3227,12 @@
       <c r="K22" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L22" s="112" t="str">
+      <c r="L22" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="17.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>8</v>
       </c>
@@ -3254,12 +3252,12 @@
       <c r="K23" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L23" s="112" t="str">
+      <c r="L23" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" s="84" customFormat="1" ht="166.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="78" t="s">
         <v>8</v>
       </c>
@@ -3285,12 +3283,12 @@
       <c r="K24" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L24" s="112" t="str">
+      <c r="L24" s="9" t="str">
         <f t="shared" si="0"/>
         <v>100%</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" s="84" customFormat="1" ht="166.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="78" t="s">
         <v>8</v>
       </c>
@@ -3316,12 +3314,12 @@
       <c r="K25" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L25" s="112" t="str">
+      <c r="L25" s="9" t="str">
         <f t="shared" si="0"/>
         <v>100%</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>8</v>
       </c>
@@ -3341,12 +3339,12 @@
       <c r="K26" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L26" s="112" t="str">
+      <c r="L26" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="36.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>8</v>
       </c>
@@ -3368,12 +3366,12 @@
       <c r="K27" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L27" s="112" t="str">
+      <c r="L27" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>8</v>
       </c>
@@ -3395,12 +3393,12 @@
       <c r="K28" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L28" s="112" t="str">
+      <c r="L28" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>8</v>
       </c>
@@ -3422,12 +3420,12 @@
       <c r="K29" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L29" s="112" t="str">
+      <c r="L29" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>8</v>
       </c>
@@ -3449,12 +3447,12 @@
       <c r="K30" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L30" s="112" t="str">
+      <c r="L30" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="56.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>8</v>
       </c>
@@ -3478,12 +3476,12 @@
       <c r="K31" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L31" s="112" t="str">
+      <c r="L31" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="20.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>8</v>
       </c>
@@ -3505,12 +3503,12 @@
       <c r="K32" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L32" s="112" t="str">
+      <c r="L32" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="20.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>8</v>
       </c>
@@ -3530,12 +3528,12 @@
       <c r="K33" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L33" s="112" t="str">
+      <c r="L33" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="20.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>8</v>
       </c>
@@ -3555,12 +3553,12 @@
       <c r="K34" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L34" s="112" t="str">
+      <c r="L34" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="20.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>8</v>
       </c>
@@ -3580,12 +3578,12 @@
       <c r="K35" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L35" s="112" t="str">
+      <c r="L35" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="69.650000000000006" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>8</v>
       </c>
@@ -3609,12 +3607,12 @@
       <c r="K36" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L36" s="112" t="str">
+      <c r="L36" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="22" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" s="22" customFormat="1" ht="26.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
         <v>8</v>
       </c>
@@ -3638,12 +3636,12 @@
       <c r="K37" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L37" s="112" t="str">
+      <c r="L37" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="22.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>8</v>
       </c>
@@ -3665,12 +3663,12 @@
       <c r="K38" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L38" s="112" t="str">
+      <c r="L38" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>8</v>
       </c>
@@ -3694,12 +3692,12 @@
       <c r="K39" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L39" s="112" t="str">
+      <c r="L39" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="20.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
         <v>8</v>
       </c>
@@ -3721,12 +3719,12 @@
       <c r="K40" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L40" s="112" t="str">
+      <c r="L40" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="19.399999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
         <v>8</v>
       </c>
@@ -3748,12 +3746,12 @@
       <c r="K41" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L41" s="112" t="str">
+      <c r="L41" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="36.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>8</v>
       </c>
@@ -3775,12 +3773,12 @@
       <c r="K42" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L42" s="112" t="str">
+      <c r="L42" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="26.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="26.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>8</v>
       </c>
@@ -3802,12 +3800,12 @@
       <c r="K43" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L43" s="112" t="str">
+      <c r="L43" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="46.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="46.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
         <v>8</v>
       </c>
@@ -3829,12 +3827,12 @@
       <c r="K44" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L44" s="112" t="str">
+      <c r="L44" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" ht="27.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>8</v>
       </c>
@@ -3854,12 +3852,12 @@
       <c r="K45" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L45" s="112" t="str">
+      <c r="L45" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>8</v>
       </c>
@@ -3881,12 +3879,12 @@
       <c r="K46" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L46" s="112" t="str">
+      <c r="L46" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" s="30" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>8</v>
       </c>
@@ -3908,12 +3906,12 @@
       <c r="K47" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L47" s="112" t="str">
+      <c r="L47" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="30" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" s="30" customFormat="1" ht="32.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>8</v>
       </c>
@@ -3935,12 +3933,12 @@
       <c r="K48" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L48" s="112" t="str">
+      <c r="L48" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" s="30" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>8</v>
       </c>
@@ -3962,12 +3960,12 @@
       <c r="K49" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L49" s="112" t="str">
+      <c r="L49" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="30" customFormat="1" ht="71.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" s="30" customFormat="1" ht="71.150000000000006" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>8</v>
       </c>
@@ -3989,12 +3987,12 @@
       <c r="K50" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L50" s="112" t="str">
+      <c r="L50" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" s="72" customFormat="1" ht="129" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="67" t="s">
         <v>8</v>
       </c>
@@ -4020,12 +4018,12 @@
       <c r="K51" s="72" t="s">
         <v>270</v>
       </c>
-      <c r="L51" s="112" t="str">
+      <c r="L51" s="9" t="str">
         <f t="shared" si="0"/>
         <v>50%</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" s="72" customFormat="1" ht="129" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="67" t="s">
         <v>8</v>
       </c>
@@ -4051,12 +4049,12 @@
       <c r="K52" s="72" t="s">
         <v>270</v>
       </c>
-      <c r="L52" s="112" t="str">
+      <c r="L52" s="9" t="str">
         <f t="shared" si="0"/>
         <v>50%</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" s="72" customFormat="1" ht="129" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="67" t="s">
         <v>8</v>
       </c>
@@ -4082,12 +4080,12 @@
       <c r="K53" s="72" t="s">
         <v>270</v>
       </c>
-      <c r="L53" s="112" t="str">
+      <c r="L53" s="9" t="str">
         <f t="shared" si="0"/>
         <v>50%</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>8</v>
       </c>
@@ -4109,12 +4107,12 @@
       <c r="K54" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L54" s="112" t="str">
+      <c r="L54" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="84" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" s="84" customFormat="1" ht="94" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="78" t="s">
         <v>8</v>
       </c>
@@ -4138,12 +4136,12 @@
       <c r="K55" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L55" s="112" t="str">
+      <c r="L55" s="9" t="str">
         <f t="shared" si="0"/>
         <v>100%</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" ht="17.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>8</v>
       </c>
@@ -4163,12 +4161,12 @@
       <c r="K56" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L56" s="112" t="str">
+      <c r="L56" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>8</v>
       </c>
@@ -4190,12 +4188,12 @@
       <c r="K57" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L57" s="112" t="str">
+      <c r="L57" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="24.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>8</v>
       </c>
@@ -4215,12 +4213,12 @@
       <c r="K58" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L58" s="112" t="str">
+      <c r="L58" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" ht="24.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>8</v>
       </c>
@@ -4240,12 +4238,12 @@
       <c r="K59" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L59" s="112" t="str">
+      <c r="L59" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
         <v>8</v>
       </c>
@@ -4267,12 +4265,12 @@
       <c r="K60" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L60" s="112" t="str">
+      <c r="L60" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" ht="21.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>8</v>
       </c>
@@ -4292,12 +4290,12 @@
       <c r="K61" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L61" s="112" t="str">
+      <c r="L61" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="23.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" ht="23.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
         <v>8</v>
       </c>
@@ -4318,12 +4316,12 @@
       <c r="K62" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L62" s="112" t="str">
+      <c r="L62" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>8</v>
       </c>
@@ -4345,12 +4343,12 @@
       <c r="K63" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L63" s="112" t="str">
+      <c r="L63" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>8</v>
       </c>
@@ -4372,12 +4370,12 @@
       <c r="K64" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L64" s="112" t="str">
+      <c r="L64" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>8</v>
       </c>
@@ -4396,12 +4394,12 @@
       <c r="K65" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L65" s="112" t="str">
+      <c r="L65" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>8</v>
       </c>
@@ -4421,12 +4419,12 @@
       <c r="K66" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L66" s="112" t="str">
+      <c r="L66" s="9" t="str">
         <f t="shared" si="0"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>8</v>
       </c>
@@ -4448,12 +4446,12 @@
       <c r="K67" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L67" s="112" t="str">
+      <c r="L67" s="9" t="str">
         <f t="shared" ref="L67:L130" si="1">IF(K67="Yellow", "50%", IF(K67="Green", "100%", IF(K67="Grey", "0%", IF(K67="White", "30%", IF(K67="Orange", "10%", "")))))</f>
         <v>30%</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
         <v>8</v>
       </c>
@@ -4473,12 +4471,12 @@
       <c r="K68" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L68" s="112" t="str">
+      <c r="L68" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" ht="30.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>8</v>
       </c>
@@ -4500,12 +4498,12 @@
       <c r="K69" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L69" s="112" t="str">
+      <c r="L69" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>8</v>
       </c>
@@ -4527,12 +4525,12 @@
       <c r="K70" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L70" s="112" t="str">
+      <c r="L70" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" ht="32.15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
         <v>8</v>
       </c>
@@ -4554,12 +4552,12 @@
       <c r="K71" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L71" s="112" t="str">
+      <c r="L71" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>8</v>
       </c>
@@ -4583,12 +4581,12 @@
       <c r="K72" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L72" s="112" t="str">
+      <c r="L72" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>8</v>
       </c>
@@ -4612,12 +4610,12 @@
       <c r="K73" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L73" s="112" t="str">
+      <c r="L73" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>8</v>
       </c>
@@ -4639,12 +4637,12 @@
       <c r="K74" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L74" s="112" t="str">
+      <c r="L74" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>8</v>
       </c>
@@ -4664,12 +4662,12 @@
       <c r="K75" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L75" s="112" t="str">
+      <c r="L75" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" ht="68.150000000000006" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
         <v>8</v>
       </c>
@@ -4689,12 +4687,12 @@
       <c r="K76" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L76" s="112" t="str">
+      <c r="L76" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
         <v>8</v>
       </c>
@@ -4714,12 +4712,12 @@
       <c r="K77" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L77" s="112" t="str">
+      <c r="L77" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" ht="35.15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="s">
         <v>8</v>
       </c>
@@ -4739,12 +4737,12 @@
       <c r="K78" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L78" s="112" t="str">
+      <c r="L78" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
         <v>8</v>
       </c>
@@ -4764,12 +4762,12 @@
       <c r="K79" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L79" s="112" t="str">
+      <c r="L79" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="s">
         <v>8</v>
       </c>
@@ -4789,12 +4787,12 @@
       <c r="K80" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L80" s="112" t="str">
+      <c r="L80" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="10" t="s">
         <v>8</v>
       </c>
@@ -4814,12 +4812,12 @@
       <c r="K81" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L81" s="112" t="str">
+      <c r="L81" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" ht="36.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="10" t="s">
         <v>8</v>
       </c>
@@ -4839,12 +4837,12 @@
       <c r="K82" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L82" s="112" t="str">
+      <c r="L82" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="10" t="s">
         <v>8</v>
       </c>
@@ -4864,12 +4862,12 @@
       <c r="K83" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L83" s="112" t="str">
+      <c r="L83" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="10" t="s">
         <v>8</v>
       </c>
@@ -4889,12 +4887,12 @@
       <c r="K84" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L84" s="112" t="str">
+      <c r="L84" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="63" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" s="63" customFormat="1" ht="61.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="64" t="s">
         <v>8</v>
       </c>
@@ -4920,12 +4918,12 @@
       <c r="K85" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L85" s="112" t="str">
+      <c r="L85" s="9" t="str">
         <f t="shared" si="1"/>
         <v>50%</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" ht="35.15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="10" t="s">
         <v>8</v>
       </c>
@@ -4945,12 +4943,12 @@
       <c r="K86" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L86" s="112" t="str">
+      <c r="L86" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="87" spans="1:12" s="63" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" s="63" customFormat="1" ht="79" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="s">
         <v>8</v>
       </c>
@@ -4976,12 +4974,12 @@
       <c r="K87" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L87" s="112" t="str">
+      <c r="L87" s="9" t="str">
         <f t="shared" si="1"/>
         <v>50%</v>
       </c>
     </row>
-    <row r="88" spans="1:12" s="63" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" s="63" customFormat="1" ht="79" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="s">
         <v>8</v>
       </c>
@@ -5007,12 +5005,12 @@
       <c r="K88" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L88" s="112" t="str">
+      <c r="L88" s="9" t="str">
         <f t="shared" si="1"/>
         <v>50%</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" ht="27.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="10" t="s">
         <v>8</v>
       </c>
@@ -5032,12 +5030,12 @@
       <c r="K89" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L89" s="112" t="str">
+      <c r="L89" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="10" t="s">
         <v>8</v>
       </c>
@@ -5057,12 +5055,12 @@
       <c r="K90" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L90" s="112" t="str">
+      <c r="L90" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="10" t="s">
         <v>8</v>
       </c>
@@ -5082,12 +5080,12 @@
       <c r="K91" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L91" s="112" t="str">
+      <c r="L91" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" ht="15.65" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="10" t="s">
         <v>8</v>
       </c>
@@ -5107,12 +5105,12 @@
       <c r="K92" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L92" s="112" t="str">
+      <c r="L92" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" ht="41.15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="10" t="s">
         <v>8</v>
       </c>
@@ -5132,12 +5130,12 @@
       <c r="K93" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L93" s="112" t="str">
+      <c r="L93" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="10" t="s">
         <v>8</v>
       </c>
@@ -5157,12 +5155,12 @@
       <c r="K94" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L94" s="112" t="str">
+      <c r="L94" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="10" t="s">
         <v>8</v>
       </c>
@@ -5182,12 +5180,12 @@
       <c r="K95" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L95" s="112" t="str">
+      <c r="L95" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" ht="20.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="10" t="s">
         <v>8</v>
       </c>
@@ -5207,12 +5205,12 @@
       <c r="K96" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L96" s="112" t="str">
+      <c r="L96" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" ht="52.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
         <v>8</v>
       </c>
@@ -5234,12 +5232,12 @@
       <c r="K97" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L97" s="112" t="str">
+      <c r="L97" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
         <v>8</v>
       </c>
@@ -5259,12 +5257,12 @@
       <c r="K98" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L98" s="112" t="str">
+      <c r="L98" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" ht="37.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10" t="s">
         <v>8</v>
       </c>
@@ -5284,12 +5282,12 @@
       <c r="K99" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L99" s="112" t="str">
+      <c r="L99" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" ht="37.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="10" t="s">
         <v>8</v>
       </c>
@@ -5309,12 +5307,12 @@
       <c r="K100" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L100" s="112" t="str">
+      <c r="L100" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" ht="23.15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="s">
         <v>8</v>
       </c>
@@ -5333,12 +5331,12 @@
       <c r="K101" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L101" s="112" t="str">
+      <c r="L101" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="10" t="s">
         <v>8</v>
       </c>
@@ -5360,12 +5358,12 @@
       <c r="K102" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L102" s="112" t="str">
+      <c r="L102" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="10" t="s">
         <v>8</v>
       </c>
@@ -5385,12 +5383,12 @@
       <c r="K103" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L103" s="112" t="str">
+      <c r="L103" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" ht="22.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="10" t="s">
         <v>8</v>
       </c>
@@ -5412,12 +5410,12 @@
       <c r="K104" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L104" s="112" t="str">
+      <c r="L104" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" ht="22.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10" t="s">
         <v>8</v>
       </c>
@@ -5437,12 +5435,12 @@
       <c r="K105" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L105" s="112" t="str">
+      <c r="L105" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" ht="22.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="10" t="s">
         <v>8</v>
       </c>
@@ -5462,12 +5460,12 @@
       <c r="K106" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L106" s="112" t="str">
+      <c r="L106" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" ht="22.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="s">
         <v>8</v>
       </c>
@@ -5487,12 +5485,12 @@
       <c r="K107" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L107" s="112" t="str">
+      <c r="L107" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="10" t="s">
         <v>8</v>
       </c>
@@ -5516,12 +5514,12 @@
       <c r="K108" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L108" s="112" t="str">
+      <c r="L108" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
         <v>8</v>
       </c>
@@ -5543,12 +5541,12 @@
       <c r="K109" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L109" s="112" t="str">
+      <c r="L109" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="10" t="s">
         <v>8</v>
       </c>
@@ -5568,12 +5566,12 @@
       <c r="K110" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L110" s="112" t="str">
+      <c r="L110" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="10" t="s">
         <v>8</v>
       </c>
@@ -5593,12 +5591,12 @@
       <c r="K111" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L111" s="112" t="str">
+      <c r="L111" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="10" t="s">
         <v>8</v>
       </c>
@@ -5620,12 +5618,12 @@
       <c r="K112" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L112" s="112" t="str">
+      <c r="L112" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="10" t="s">
         <v>8</v>
       </c>
@@ -5647,12 +5645,12 @@
       <c r="K113" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L113" s="112" t="str">
+      <c r="L113" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="s">
         <v>8</v>
       </c>
@@ -5674,12 +5672,12 @@
       <c r="K114" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L114" s="112" t="str">
+      <c r="L114" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="s">
         <v>8</v>
       </c>
@@ -5701,12 +5699,12 @@
       <c r="K115" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L115" s="112" t="str">
+      <c r="L115" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="10" t="s">
         <v>8</v>
       </c>
@@ -5728,12 +5726,12 @@
       <c r="K116" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L116" s="112" t="str">
+      <c r="L116" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" ht="103" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="10" t="s">
         <v>8</v>
       </c>
@@ -5757,12 +5755,12 @@
       <c r="K117" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L117" s="112" t="str">
+      <c r="L117" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="84" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" s="84" customFormat="1" ht="178.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="78" t="s">
         <v>8</v>
       </c>
@@ -5788,12 +5786,12 @@
       <c r="K118" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L118" s="112" t="str">
+      <c r="L118" s="9" t="str">
         <f t="shared" si="1"/>
         <v>100%</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" ht="54" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="10" t="s">
         <v>8</v>
       </c>
@@ -5815,12 +5813,12 @@
       <c r="K119" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L119" s="112" t="str">
+      <c r="L119" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" ht="54" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="10" t="s">
         <v>8</v>
       </c>
@@ -5842,12 +5840,12 @@
       <c r="K120" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L120" s="112" t="str">
+      <c r="L120" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" ht="54" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="10" t="s">
         <v>8</v>
       </c>
@@ -5869,12 +5867,12 @@
       <c r="K121" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L121" s="112" t="str">
+      <c r="L121" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="122" spans="1:12" s="63" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" s="63" customFormat="1" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="64" t="s">
         <v>8</v>
       </c>
@@ -5900,12 +5898,12 @@
       <c r="K122" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L122" s="112" t="str">
+      <c r="L122" s="9" t="str">
         <f t="shared" si="1"/>
         <v>50%</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="31.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" ht="31.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="19" t="s">
         <v>8</v>
       </c>
@@ -5923,12 +5921,12 @@
       <c r="K123" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L123" s="112" t="str">
+      <c r="L123" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="19" t="s">
         <v>8</v>
       </c>
@@ -5948,12 +5946,12 @@
       <c r="K124" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L124" s="112" t="str">
+      <c r="L124" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="19" t="s">
         <v>8</v>
       </c>
@@ -5973,12 +5971,12 @@
       <c r="K125" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L125" s="112" t="str">
+      <c r="L125" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="19" t="s">
         <v>8</v>
       </c>
@@ -5998,12 +5996,12 @@
       <c r="K126" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L126" s="112" t="str">
+      <c r="L126" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="19" t="s">
         <v>8</v>
       </c>
@@ -6023,12 +6021,12 @@
       <c r="K127" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L127" s="112" t="str">
+      <c r="L127" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="19" t="s">
         <v>8</v>
       </c>
@@ -6048,12 +6046,12 @@
       <c r="K128" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L128" s="112" t="str">
+      <c r="L128" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="10" t="s">
         <v>78</v>
       </c>
@@ -6075,12 +6073,12 @@
       <c r="K129" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L129" s="112" t="str">
+      <c r="L129" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="10" t="s">
         <v>78</v>
       </c>
@@ -6100,12 +6098,12 @@
       <c r="K130" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L130" s="112" t="str">
+      <c r="L130" s="9" t="str">
         <f t="shared" si="1"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="10" t="s">
         <v>78</v>
       </c>
@@ -6127,12 +6125,12 @@
       <c r="K131" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L131" s="112" t="str">
+      <c r="L131" s="9" t="str">
         <f t="shared" ref="L131:L194" si="2">IF(K131="Yellow", "50%", IF(K131="Green", "100%", IF(K131="Grey", "0%", IF(K131="White", "30%", IF(K131="Orange", "10%", "")))))</f>
         <v>30%</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="10" t="s">
         <v>78</v>
       </c>
@@ -6156,12 +6154,12 @@
       <c r="K132" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L132" s="112" t="str">
+      <c r="L132" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="10" t="s">
         <v>78</v>
       </c>
@@ -6183,12 +6181,12 @@
       <c r="K133" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L133" s="112" t="str">
+      <c r="L133" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="10" t="s">
         <v>78</v>
       </c>
@@ -6210,12 +6208,12 @@
       <c r="K134" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L134" s="112" t="str">
+      <c r="L134" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="10" t="s">
         <v>78</v>
       </c>
@@ -6239,12 +6237,12 @@
       <c r="K135" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L135" s="112" t="str">
+      <c r="L135" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="10" t="s">
         <v>78</v>
       </c>
@@ -6268,12 +6266,12 @@
       <c r="K136" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L136" s="112" t="str">
+      <c r="L136" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="10" t="s">
         <v>78</v>
       </c>
@@ -6295,12 +6293,12 @@
       <c r="K137" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L137" s="112" t="str">
+      <c r="L137" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="10" t="s">
         <v>78</v>
       </c>
@@ -6322,12 +6320,12 @@
       <c r="K138" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L138" s="112" t="str">
+      <c r="L138" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="10" t="s">
         <v>78</v>
       </c>
@@ -6349,12 +6347,12 @@
       <c r="K139" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L139" s="112" t="str">
+      <c r="L139" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="10" t="s">
         <v>78</v>
       </c>
@@ -6376,12 +6374,12 @@
       <c r="K140" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L140" s="112" t="str">
+      <c r="L140" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="10" t="s">
         <v>78</v>
       </c>
@@ -6401,12 +6399,12 @@
       <c r="K141" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L141" s="112" t="str">
+      <c r="L141" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="10" t="s">
         <v>78</v>
       </c>
@@ -6430,12 +6428,12 @@
       <c r="K142" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L142" s="112" t="str">
+      <c r="L142" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="10" t="s">
         <v>78</v>
       </c>
@@ -6457,12 +6455,12 @@
       <c r="K143" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L143" s="112" t="str">
+      <c r="L143" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="25" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="10" t="s">
         <v>78</v>
       </c>
@@ -6484,12 +6482,12 @@
       <c r="K144" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L144" s="112" t="str">
+      <c r="L144" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="10" t="s">
         <v>78</v>
       </c>
@@ -6513,12 +6511,12 @@
       <c r="K145" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L145" s="112" t="str">
+      <c r="L145" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="10" t="s">
         <v>78</v>
       </c>
@@ -6542,12 +6540,12 @@
       <c r="K146" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L146" s="112" t="str">
+      <c r="L146" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="10" t="s">
         <v>78</v>
       </c>
@@ -6571,12 +6569,12 @@
       <c r="K147" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L147" s="112" t="str">
+      <c r="L147" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="10" t="s">
         <v>78</v>
       </c>
@@ -6598,12 +6596,12 @@
       <c r="K148" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L148" s="112" t="str">
+      <c r="L148" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="10" t="s">
         <v>78</v>
       </c>
@@ -6623,12 +6621,12 @@
       <c r="K149" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L149" s="112" t="str">
+      <c r="L149" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="10" t="s">
         <v>78</v>
       </c>
@@ -6650,12 +6648,12 @@
       <c r="K150" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L150" s="112" t="str">
+      <c r="L150" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="10" t="s">
         <v>78</v>
       </c>
@@ -6677,12 +6675,12 @@
       <c r="K151" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L151" s="112" t="str">
+      <c r="L151" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="10" t="s">
         <v>78</v>
       </c>
@@ -6704,12 +6702,12 @@
       <c r="K152" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L152" s="112" t="str">
+      <c r="L152" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="10" t="s">
         <v>78</v>
       </c>
@@ -6731,12 +6729,12 @@
       <c r="K153" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L153" s="112" t="str">
+      <c r="L153" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="10" t="s">
         <v>78</v>
       </c>
@@ -6758,12 +6756,12 @@
       <c r="K154" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L154" s="112" t="str">
+      <c r="L154" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" s="10" t="s">
         <v>78</v>
       </c>
@@ -6785,12 +6783,12 @@
       <c r="K155" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L155" s="112" t="str">
+      <c r="L155" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" s="10" t="s">
         <v>78</v>
       </c>
@@ -6812,12 +6810,12 @@
       <c r="K156" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L156" s="112" t="str">
+      <c r="L156" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" s="10" t="s">
         <v>78</v>
       </c>
@@ -6839,12 +6837,12 @@
       <c r="K157" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L157" s="112" t="str">
+      <c r="L157" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="10" t="s">
         <v>78</v>
       </c>
@@ -6866,12 +6864,12 @@
       <c r="K158" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L158" s="112" t="str">
+      <c r="L158" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="10" t="s">
         <v>78</v>
       </c>
@@ -6893,12 +6891,12 @@
       <c r="K159" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L159" s="112" t="str">
+      <c r="L159" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="85" t="s">
         <v>78</v>
       </c>
@@ -6924,13 +6922,13 @@
       <c r="K160" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="L160" s="112" t="str">
+      <c r="L160" s="9" t="str">
         <f t="shared" si="2"/>
         <v>10%</v>
       </c>
       <c r="M160" s="93"/>
     </row>
-    <row r="161" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="10" t="s">
         <v>78</v>
       </c>
@@ -6954,12 +6952,12 @@
       <c r="K161" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L161" s="112" t="str">
+      <c r="L161" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" s="10" t="s">
         <v>78</v>
       </c>
@@ -6979,12 +6977,12 @@
       <c r="K162" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L162" s="112" t="str">
+      <c r="L162" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" s="10" t="s">
         <v>78</v>
       </c>
@@ -7004,12 +7002,12 @@
       <c r="K163" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L163" s="112" t="str">
+      <c r="L163" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="10" t="s">
         <v>78</v>
       </c>
@@ -7029,12 +7027,12 @@
       <c r="K164" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L164" s="112" t="str">
+      <c r="L164" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="10" t="s">
         <v>78</v>
       </c>
@@ -7054,12 +7052,12 @@
       <c r="K165" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L165" s="112" t="str">
+      <c r="L165" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="10" t="s">
         <v>78</v>
       </c>
@@ -7079,12 +7077,12 @@
       <c r="K166" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L166" s="112" t="str">
+      <c r="L166" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" ht="38.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" s="78" t="s">
         <v>78</v>
       </c>
@@ -7110,13 +7108,13 @@
       <c r="K167" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L167" s="112" t="str">
+      <c r="L167" s="9" t="str">
         <f t="shared" si="2"/>
         <v>100%</v>
       </c>
       <c r="M167" s="84"/>
     </row>
-    <row r="168" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="10" t="s">
         <v>78</v>
       </c>
@@ -7140,12 +7138,12 @@
       <c r="K168" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L168" s="112" t="str">
+      <c r="L168" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" s="10" t="s">
         <v>78</v>
       </c>
@@ -7169,12 +7167,12 @@
       <c r="K169" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L169" s="112" t="str">
+      <c r="L169" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="10" t="s">
         <v>78</v>
       </c>
@@ -7198,12 +7196,12 @@
       <c r="K170" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L170" s="112" t="str">
+      <c r="L170" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" s="10" t="s">
         <v>78</v>
       </c>
@@ -7227,12 +7225,12 @@
       <c r="K171" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L171" s="112" t="str">
+      <c r="L171" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="38.5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:13" ht="38.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="78" t="s">
         <v>78</v>
       </c>
@@ -7258,13 +7256,13 @@
       <c r="K172" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L172" s="112" t="str">
+      <c r="L172" s="9" t="str">
         <f t="shared" si="2"/>
         <v>100%</v>
       </c>
       <c r="M172" s="84"/>
     </row>
-    <row r="173" spans="1:13" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:13" ht="37.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="85" t="s">
         <v>78</v>
       </c>
@@ -7290,13 +7288,13 @@
       <c r="K173" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="L173" s="112" t="str">
+      <c r="L173" s="9" t="str">
         <f t="shared" si="2"/>
         <v>10%</v>
       </c>
       <c r="M173" s="93"/>
     </row>
-    <row r="174" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="10" t="s">
         <v>78</v>
       </c>
@@ -7318,12 +7316,12 @@
       <c r="K174" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L174" s="112" t="str">
+      <c r="L174" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" s="10" t="s">
         <v>78</v>
       </c>
@@ -7345,12 +7343,12 @@
       <c r="K175" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L175" s="112" t="str">
+      <c r="L175" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="s">
         <v>78</v>
       </c>
@@ -7372,12 +7370,12 @@
       <c r="K176" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L176" s="112" t="str">
+      <c r="L176" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" ht="37.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="10" t="s">
         <v>78</v>
       </c>
@@ -7399,12 +7397,12 @@
       <c r="K177" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L177" s="112" t="str">
+      <c r="L177" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="10" t="s">
         <v>78</v>
       </c>
@@ -7426,12 +7424,12 @@
       <c r="K178" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L178" s="112" t="str">
+      <c r="L178" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="10" t="s">
         <v>78</v>
       </c>
@@ -7453,12 +7451,12 @@
       <c r="K179" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L179" s="112" t="str">
+      <c r="L179" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="10" t="s">
         <v>78</v>
       </c>
@@ -7480,12 +7478,12 @@
       <c r="K180" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L180" s="112" t="str">
+      <c r="L180" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="10" t="s">
         <v>78</v>
       </c>
@@ -7507,12 +7505,12 @@
       <c r="K181" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L181" s="112" t="str">
+      <c r="L181" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="10" t="s">
         <v>78</v>
       </c>
@@ -7534,12 +7532,12 @@
       <c r="K182" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L182" s="112" t="str">
+      <c r="L182" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="183" spans="1:13" ht="64.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" ht="64.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="64" t="s">
         <v>78</v>
       </c>
@@ -7565,13 +7563,13 @@
       <c r="K183" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L183" s="112" t="str">
+      <c r="L183" s="9" t="str">
         <f t="shared" si="2"/>
         <v>50%</v>
       </c>
       <c r="M183" s="63"/>
     </row>
-    <row r="184" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="10" t="s">
         <v>95</v>
       </c>
@@ -7591,12 +7589,12 @@
       <c r="K184" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L184" s="112" t="str">
+      <c r="L184" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="10" t="s">
         <v>95</v>
       </c>
@@ -7616,12 +7614,12 @@
       <c r="K185" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L185" s="112" t="str">
+      <c r="L185" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="10" t="s">
         <v>95</v>
       </c>
@@ -7641,12 +7639,12 @@
       <c r="K186" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L186" s="112" t="str">
+      <c r="L186" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="10" t="s">
         <v>95</v>
       </c>
@@ -7666,12 +7664,12 @@
       <c r="K187" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L187" s="112" t="str">
+      <c r="L187" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="10" t="s">
         <v>95</v>
       </c>
@@ -7691,12 +7689,12 @@
       <c r="K188" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L188" s="112" t="str">
+      <c r="L188" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="10" t="s">
         <v>95</v>
       </c>
@@ -7716,12 +7714,12 @@
       <c r="K189" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L189" s="112" t="str">
+      <c r="L189" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="10" t="s">
         <v>95</v>
       </c>
@@ -7739,12 +7737,12 @@
       <c r="K190" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L190" s="112" t="str">
+      <c r="L190" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="10" t="s">
         <v>95</v>
       </c>
@@ -7764,12 +7762,12 @@
       <c r="K191" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L191" s="112" t="str">
+      <c r="L191" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" s="10" t="s">
         <v>100</v>
       </c>
@@ -7789,12 +7787,12 @@
       <c r="K192" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L192" s="112" t="str">
+      <c r="L192" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" s="10" t="s">
         <v>100</v>
       </c>
@@ -7814,12 +7812,12 @@
       <c r="K193" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L193" s="112" t="str">
+      <c r="L193" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" s="10" t="s">
         <v>100</v>
       </c>
@@ -7841,12 +7839,12 @@
       <c r="K194" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L194" s="112" t="str">
+      <c r="L194" s="9" t="str">
         <f t="shared" si="2"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="195" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="10" t="s">
         <v>100</v>
       </c>
@@ -7866,12 +7864,12 @@
       <c r="K195" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L195" s="112" t="str">
-        <f t="shared" ref="L195:L232" si="3">IF(K195="Yellow", "50%", IF(K195="Green", "100%", IF(K195="Grey", "0%", IF(K195="White", "30%", IF(K195="Orange", "10%", "")))))</f>
-        <v>30%</v>
-      </c>
-    </row>
-    <row r="196" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+      <c r="L195" s="9" t="str">
+        <f t="shared" ref="L195:L231" si="3">IF(K195="Yellow", "50%", IF(K195="Green", "100%", IF(K195="Grey", "0%", IF(K195="White", "30%", IF(K195="Orange", "10%", "")))))</f>
+        <v>30%</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" s="10" t="s">
         <v>100</v>
       </c>
@@ -7891,12 +7889,12 @@
       <c r="K196" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L196" s="112" t="str">
+      <c r="L196" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" s="10" t="s">
         <v>100</v>
       </c>
@@ -7916,12 +7914,12 @@
       <c r="K197" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L197" s="112" t="str">
+      <c r="L197" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" s="10" t="s">
         <v>100</v>
       </c>
@@ -7939,12 +7937,12 @@
       <c r="K198" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L198" s="112" t="str">
+      <c r="L198" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" s="10" t="s">
         <v>100</v>
       </c>
@@ -7964,12 +7962,12 @@
       <c r="K199" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L199" s="112" t="str">
+      <c r="L199" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" s="10" t="s">
         <v>100</v>
       </c>
@@ -7989,12 +7987,12 @@
       <c r="K200" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L200" s="112" t="str">
+      <c r="L200" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" s="10" t="s">
         <v>100</v>
       </c>
@@ -8014,12 +8012,12 @@
       <c r="K201" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L201" s="112" t="str">
+      <c r="L201" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" s="10" t="s">
         <v>100</v>
       </c>
@@ -8039,12 +8037,12 @@
       <c r="K202" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L202" s="112" t="str">
+      <c r="L202" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" s="10" t="s">
         <v>100</v>
       </c>
@@ -8066,13 +8064,13 @@
       <c r="K203" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L203" s="112" t="str">
+      <c r="L203" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
       <c r="M203" s="45"/>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="10" t="s">
         <v>100</v>
       </c>
@@ -8090,12 +8088,12 @@
       <c r="K204" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L204" s="112" t="str">
+      <c r="L204" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="10" t="s">
         <v>100</v>
       </c>
@@ -8113,12 +8111,12 @@
       <c r="K205" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L205" s="112" t="str">
+      <c r="L205" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" s="10" t="s">
         <v>100</v>
       </c>
@@ -8136,12 +8134,12 @@
       <c r="K206" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L206" s="112" t="str">
+      <c r="L206" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="10" t="s">
         <v>100</v>
       </c>
@@ -8161,12 +8159,12 @@
       <c r="K207" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L207" s="112" t="str">
+      <c r="L207" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:13" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" s="64" t="s">
         <v>100</v>
       </c>
@@ -8190,13 +8188,13 @@
       <c r="K208" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L208" s="112" t="str">
+      <c r="L208" s="9" t="str">
         <f t="shared" si="3"/>
         <v>50%</v>
       </c>
       <c r="M208" s="63"/>
     </row>
-    <row r="209" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:13" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="64" t="s">
         <v>100</v>
       </c>
@@ -8220,13 +8218,13 @@
       <c r="K209" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L209" s="112" t="str">
+      <c r="L209" s="9" t="str">
         <f t="shared" si="3"/>
         <v>50%</v>
       </c>
       <c r="M209" s="63"/>
     </row>
-    <row r="210" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:13" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" s="64" t="s">
         <v>100</v>
       </c>
@@ -8250,13 +8248,13 @@
       <c r="K210" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L210" s="112" t="str">
+      <c r="L210" s="9" t="str">
         <f t="shared" si="3"/>
         <v>50%</v>
       </c>
       <c r="M210" s="63"/>
     </row>
-    <row r="211" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:13" ht="409.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="64" t="s">
         <v>100</v>
       </c>
@@ -8280,13 +8278,13 @@
       <c r="K211" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L211" s="112" t="str">
+      <c r="L211" s="9" t="str">
         <f t="shared" si="3"/>
         <v>50%</v>
       </c>
       <c r="M211" s="63"/>
     </row>
-    <row r="212" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:13" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="64" t="s">
         <v>100</v>
       </c>
@@ -8306,13 +8304,13 @@
       <c r="K212" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L212" s="112" t="str">
+      <c r="L212" s="9" t="str">
         <f t="shared" si="3"/>
         <v>50%</v>
       </c>
       <c r="M212" s="63"/>
     </row>
-    <row r="213" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:13" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="64" t="s">
         <v>100</v>
       </c>
@@ -8332,13 +8330,13 @@
       <c r="K213" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L213" s="112" t="str">
+      <c r="L213" s="9" t="str">
         <f t="shared" si="3"/>
         <v>50%</v>
       </c>
       <c r="M213" s="63"/>
     </row>
-    <row r="214" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:13" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" s="64" t="s">
         <v>100</v>
       </c>
@@ -8358,13 +8356,13 @@
       <c r="K214" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L214" s="112" t="str">
+      <c r="L214" s="9" t="str">
         <f t="shared" si="3"/>
         <v>50%</v>
       </c>
       <c r="M214" s="63"/>
     </row>
-    <row r="215" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:13" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" s="64" t="s">
         <v>100</v>
       </c>
@@ -8384,13 +8382,13 @@
       <c r="K215" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="L215" s="112" t="str">
+      <c r="L215" s="9" t="str">
         <f t="shared" si="3"/>
         <v>50%</v>
       </c>
       <c r="M215" s="63"/>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" s="10" t="s">
         <v>100</v>
       </c>
@@ -8414,12 +8412,12 @@
       <c r="K216" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L216" s="112" t="str">
+      <c r="L216" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" s="10" t="s">
         <v>100</v>
       </c>
@@ -8443,12 +8441,12 @@
       <c r="K217" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L217" s="112" t="str">
+      <c r="L217" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" s="10" t="s">
         <v>100</v>
       </c>
@@ -8472,12 +8470,12 @@
       <c r="K218" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L218" s="112" t="str">
+      <c r="L218" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" s="10" t="s">
         <v>100</v>
       </c>
@@ -8501,12 +8499,12 @@
       <c r="K219" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L219" s="112" t="str">
+      <c r="L219" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="25" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:13" ht="25" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" s="10" t="s">
         <v>100</v>
       </c>
@@ -8526,12 +8524,12 @@
       <c r="K220" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L220" s="112" t="str">
+      <c r="L220" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="221" spans="1:13" ht="13" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" s="10" t="s">
         <v>100</v>
       </c>
@@ -8551,12 +8549,12 @@
       <c r="K221" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L221" s="112" t="str">
+      <c r="L221" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="222" spans="1:13" ht="13" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:13" ht="13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" s="10" t="s">
         <v>100</v>
       </c>
@@ -8576,12 +8574,12 @@
       <c r="K222" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L222" s="112" t="str">
+      <c r="L222" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" s="10" t="s">
         <v>100</v>
       </c>
@@ -8603,12 +8601,12 @@
       <c r="K223" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L223" s="112" t="str">
+      <c r="L223" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="224" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:13" ht="38.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" s="84" t="s">
         <v>100</v>
       </c>
@@ -8630,13 +8628,13 @@
       <c r="K224" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L224" s="112" t="str">
+      <c r="L224" s="9" t="str">
         <f t="shared" si="3"/>
         <v>100%</v>
       </c>
       <c r="M224" s="84"/>
     </row>
-    <row r="225" spans="1:13" ht="39" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:13" ht="39" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" s="9" t="s">
         <v>100</v>
       </c>
@@ -8658,12 +8656,12 @@
       <c r="K225" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L225" s="112" t="str">
+      <c r="L225" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="226" spans="1:13" ht="51.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:13" ht="51.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" s="84" t="s">
         <v>100</v>
       </c>
@@ -8685,13 +8683,13 @@
       <c r="K226" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L226" s="112" t="str">
+      <c r="L226" s="9" t="str">
         <f t="shared" si="3"/>
         <v>100%</v>
       </c>
       <c r="M226" s="84"/>
     </row>
-    <row r="227" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:13" ht="25.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" s="9" t="s">
         <v>100</v>
       </c>
@@ -8713,12 +8711,12 @@
       <c r="K227" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L227" s="112" t="str">
+      <c r="L227" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="228" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:13" ht="38.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" s="84" t="s">
         <v>100</v>
       </c>
@@ -8740,13 +8738,13 @@
       <c r="K228" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L228" s="112" t="str">
+      <c r="L228" s="9" t="str">
         <f t="shared" si="3"/>
         <v>100%</v>
       </c>
       <c r="M228" s="84"/>
     </row>
-    <row r="229" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:13" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" s="9" t="s">
         <v>100</v>
       </c>
@@ -8766,12 +8764,12 @@
       <c r="K229" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="L229" s="112" t="str">
+      <c r="L229" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="230" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:13" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" s="84" t="s">
         <v>100</v>
       </c>
@@ -8793,13 +8791,13 @@
       <c r="K230" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L230" s="112" t="str">
+      <c r="L230" s="9" t="str">
         <f t="shared" si="3"/>
         <v>100%</v>
       </c>
       <c r="M230" s="84"/>
     </row>
-    <row r="231" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:13" ht="62.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" s="84" t="s">
         <v>100</v>
       </c>
@@ -8821,17 +8819,20 @@
       <c r="K231" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="L231" s="112" t="str">
+      <c r="L231" s="9" t="str">
         <f t="shared" si="3"/>
         <v>100%</v>
       </c>
       <c r="M231" s="84"/>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="L232" s="112"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M231" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M231" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Getting Started with Radiant"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="I71:I73">
     <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I71,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(I71,0)&lt;(WEEKDAY(TODAY())+7))</formula>

</xml_diff>

<commit_message>
updates pero andaming bugs sa tasks
updates:
per_user_test
tasks_by_color
views.py
per_user_edit_test
per_subsection_edit_test
models.py
forms.py

mga bugs kapag adding and removing document, section, subsection
</commit_message>
<xml_diff>
--- a/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
+++ b/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latticesemiconductor4-my.sharepoint.com/personal/jonathan_bunquin_latticesemi_com/Documents/Documents/GitHub/help_dashboard_django/dashboard/online_help/management/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="521" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DD4D662-C6C4-4E38-95BB-F5A322F36564}"/>
+  <xr:revisionPtr revIDLastSave="646" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BD08390-BC7E-4E2C-A7AA-4290D8184169}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025.1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="ECNs" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025.1'!$C$2:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025.1'!$A$1:$M$231</definedName>
     <definedName name="_Hlk95147257" localSheetId="0">'2025.1'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="286">
   <si>
     <t>Radiant Documentation</t>
   </si>
@@ -1566,6 +1566,9 @@
   </si>
   <si>
     <t>completion</t>
+  </si>
+  <si>
+    <t>no writer</t>
   </si>
 </sst>
 </file>
@@ -2618,26 +2621,26 @@
   <dimension ref="A1:M231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C237" sqref="C237"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="36" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="92.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="39" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="18.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="92.81640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="34.54296875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="30.54296875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="23.1796875" style="19" customWidth="1"/>
+    <col min="9" max="9" width="25.81640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" style="39" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="102.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="102.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>280</v>
       </c>
@@ -2678,7 +2681,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="63" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="63" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="57" t="s">
         <v>8</v>
       </c>
@@ -2707,7 +2710,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="63" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="63" customFormat="1" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
@@ -2736,7 +2739,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="63" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="63" customFormat="1" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="64" t="s">
         <v>8</v>
       </c>
@@ -2765,7 +2768,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -2775,7 +2778,9 @@
       <c r="C5" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
@@ -2790,7 +2795,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
@@ -2800,7 +2805,9 @@
       <c r="C6" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
@@ -2815,7 +2822,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2825,7 +2832,9 @@
       <c r="C7" s="110" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
@@ -2840,7 +2849,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -2867,7 +2876,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -2894,7 +2903,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
@@ -2904,7 +2913,9 @@
       <c r="C10" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
@@ -2919,7 +2930,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -2929,7 +2940,9 @@
       <c r="C11" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
@@ -2944,7 +2957,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -2954,7 +2967,9 @@
       <c r="C12" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
@@ -2969,7 +2984,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
@@ -2979,7 +2994,9 @@
       <c r="C13" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
@@ -2994,7 +3011,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
@@ -3004,7 +3021,9 @@
       <c r="C14" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
@@ -3019,7 +3038,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="54.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>8</v>
       </c>
@@ -3046,7 +3065,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
@@ -3073,7 +3092,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>8</v>
       </c>
@@ -3083,7 +3102,9 @@
       <c r="C17" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7"/>
@@ -3098,7 +3119,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>8</v>
       </c>
@@ -3125,7 +3146,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
@@ -3152,7 +3173,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
@@ -3179,7 +3200,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
@@ -3189,7 +3210,9 @@
       <c r="C21" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7"/>
@@ -3204,7 +3227,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>8</v>
       </c>
@@ -3231,7 +3254,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>8</v>
       </c>
@@ -3241,7 +3264,9 @@
       <c r="C23" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
@@ -3256,7 +3281,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="78" t="s">
         <v>8</v>
       </c>
@@ -3287,7 +3312,7 @@
         <v>100%</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="84" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="78" t="s">
         <v>8</v>
       </c>
@@ -3318,7 +3343,7 @@
         <v>100%</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>8</v>
       </c>
@@ -3328,7 +3353,9 @@
       <c r="C26" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="7"/>
@@ -3343,7 +3370,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>8</v>
       </c>
@@ -3370,7 +3397,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>8</v>
       </c>
@@ -3397,7 +3424,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>8</v>
       </c>
@@ -3424,7 +3451,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>8</v>
       </c>
@@ -3451,7 +3478,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>8</v>
       </c>
@@ -3480,7 +3507,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>8</v>
       </c>
@@ -3507,7 +3534,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>8</v>
       </c>
@@ -3517,7 +3544,9 @@
       <c r="C33" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="7"/>
@@ -3532,7 +3561,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>8</v>
       </c>
@@ -3542,7 +3571,9 @@
       <c r="C34" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D34" s="6"/>
+      <c r="D34" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="7"/>
@@ -3557,7 +3588,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="20.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>8</v>
       </c>
@@ -3567,7 +3598,9 @@
       <c r="C35" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="6"/>
+      <c r="D35" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="7"/>
@@ -3582,7 +3615,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>8</v>
       </c>
@@ -3611,7 +3644,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="22" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="22" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
         <v>8</v>
       </c>
@@ -3640,7 +3673,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>8</v>
       </c>
@@ -3667,7 +3700,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>8</v>
       </c>
@@ -3696,7 +3729,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
         <v>8</v>
       </c>
@@ -3723,7 +3756,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
         <v>8</v>
       </c>
@@ -3750,7 +3783,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>8</v>
       </c>
@@ -3777,7 +3810,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="26.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>8</v>
       </c>
@@ -3804,7 +3837,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="46.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="46.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
         <v>8</v>
       </c>
@@ -3831,7 +3864,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>8</v>
       </c>
@@ -3841,7 +3874,9 @@
       <c r="C45" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="D45" s="4"/>
+      <c r="D45" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="7"/>
@@ -3856,7 +3891,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>8</v>
       </c>
@@ -3883,7 +3918,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>8</v>
       </c>
@@ -3910,7 +3945,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="30" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" s="30" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>8</v>
       </c>
@@ -3937,7 +3972,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>8</v>
       </c>
@@ -3964,7 +3999,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="30" customFormat="1" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" s="30" customFormat="1" ht="71.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>8</v>
       </c>
@@ -3991,7 +4026,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="67" t="s">
         <v>8</v>
       </c>
@@ -4022,7 +4057,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="67" t="s">
         <v>8</v>
       </c>
@@ -4053,7 +4088,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" s="72" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="67" t="s">
         <v>8</v>
       </c>
@@ -4084,7 +4119,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>8</v>
       </c>
@@ -4111,7 +4146,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="84" customFormat="1" ht="93.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" s="84" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="78" t="s">
         <v>8</v>
       </c>
@@ -4140,7 +4175,7 @@
         <v>100%</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>8</v>
       </c>
@@ -4150,7 +4185,9 @@
       <c r="C56" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D56" s="4"/>
+      <c r="D56" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="7"/>
@@ -4165,7 +4202,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>8</v>
       </c>
@@ -4192,7 +4229,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>8</v>
       </c>
@@ -4202,7 +4239,9 @@
       <c r="C58" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D58" s="6"/>
+      <c r="D58" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="7"/>
@@ -4217,7 +4256,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="24.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>8</v>
       </c>
@@ -4227,7 +4266,9 @@
       <c r="C59" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D59" s="6"/>
+      <c r="D59" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="7"/>
@@ -4242,7 +4283,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
         <v>8</v>
       </c>
@@ -4269,7 +4310,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>8</v>
       </c>
@@ -4279,7 +4320,9 @@
       <c r="C61" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D61" s="4"/>
+      <c r="D61" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="7"/>
@@ -4294,7 +4337,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="23.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
         <v>8</v>
       </c>
@@ -4320,7 +4363,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>8</v>
       </c>
@@ -4347,7 +4390,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>8</v>
       </c>
@@ -4374,7 +4417,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>8</v>
       </c>
@@ -4383,6 +4426,9 @@
       </c>
       <c r="C65" s="23" t="s">
         <v>279</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -4398,7 +4444,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>8</v>
       </c>
@@ -4408,7 +4454,9 @@
       <c r="C66" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D66" s="4"/>
+      <c r="D66" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="7"/>
@@ -4423,7 +4471,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>8</v>
       </c>
@@ -4450,7 +4498,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
         <v>8</v>
       </c>
@@ -4460,7 +4508,9 @@
       <c r="C68" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D68" s="4"/>
+      <c r="D68" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E68" s="7"/>
       <c r="F68" s="18"/>
       <c r="G68" s="24"/>
@@ -4475,7 +4525,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>8</v>
       </c>
@@ -4502,7 +4552,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>8</v>
       </c>
@@ -4529,7 +4579,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
         <v>8</v>
       </c>
@@ -4556,7 +4606,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>8</v>
       </c>
@@ -4585,7 +4635,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>8</v>
       </c>
@@ -4614,7 +4664,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>8</v>
       </c>
@@ -4641,7 +4691,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>8</v>
       </c>
@@ -4651,7 +4701,9 @@
       <c r="C75" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D75" s="4"/>
+      <c r="D75" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="7"/>
@@ -4666,7 +4718,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
         <v>8</v>
       </c>
@@ -4676,7 +4728,9 @@
       <c r="C76" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D76" s="4"/>
+      <c r="D76" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
       <c r="G76" s="7"/>
@@ -4691,7 +4745,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
         <v>8</v>
       </c>
@@ -4701,7 +4755,9 @@
       <c r="C77" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D77" s="4"/>
+      <c r="D77" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
       <c r="G77" s="7"/>
@@ -4716,7 +4772,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="s">
         <v>8</v>
       </c>
@@ -4726,7 +4782,9 @@
       <c r="C78" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D78" s="4"/>
+      <c r="D78" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
       <c r="G78" s="7"/>
@@ -4741,7 +4799,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
         <v>8</v>
       </c>
@@ -4751,7 +4809,9 @@
       <c r="C79" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D79" s="4"/>
+      <c r="D79" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="7"/>
@@ -4766,7 +4826,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="s">
         <v>8</v>
       </c>
@@ -4776,7 +4836,9 @@
       <c r="C80" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D80" s="4"/>
+      <c r="D80" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
       <c r="G80" s="7"/>
@@ -4791,7 +4853,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A81" s="10" t="s">
         <v>8</v>
       </c>
@@ -4801,7 +4863,9 @@
       <c r="C81" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D81" s="4"/>
+      <c r="D81" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
       <c r="G81" s="7"/>
@@ -4816,7 +4880,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="10" t="s">
         <v>8</v>
       </c>
@@ -4826,7 +4890,9 @@
       <c r="C82" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D82" s="4"/>
+      <c r="D82" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="7"/>
@@ -4841,7 +4907,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A83" s="10" t="s">
         <v>8</v>
       </c>
@@ -4851,7 +4917,9 @@
       <c r="C83" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D83" s="4"/>
+      <c r="D83" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="7"/>
@@ -4866,7 +4934,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A84" s="10" t="s">
         <v>8</v>
       </c>
@@ -4876,7 +4944,9 @@
       <c r="C84" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D84" s="4"/>
+      <c r="D84" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="7"/>
@@ -4891,7 +4961,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="63" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" s="63" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="64" t="s">
         <v>8</v>
       </c>
@@ -4922,7 +4992,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="10" t="s">
         <v>8</v>
       </c>
@@ -4932,7 +5002,9 @@
       <c r="C86" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D86" s="4"/>
+      <c r="D86" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="7"/>
@@ -4947,7 +5019,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="87" spans="1:12" s="63" customFormat="1" ht="78.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" s="63" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="64" t="s">
         <v>8</v>
       </c>
@@ -4978,7 +5050,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="88" spans="1:12" s="63" customFormat="1" ht="78.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" s="63" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="64" t="s">
         <v>8</v>
       </c>
@@ -5009,7 +5081,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="10" t="s">
         <v>8</v>
       </c>
@@ -5019,7 +5091,9 @@
       <c r="C89" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D89" s="4"/>
+      <c r="D89" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
       <c r="G89" s="7"/>
@@ -5034,7 +5108,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A90" s="10" t="s">
         <v>8</v>
       </c>
@@ -5044,7 +5118,9 @@
       <c r="C90" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D90" s="4"/>
+      <c r="D90" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
       <c r="G90" s="7"/>
@@ -5059,7 +5135,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="10" t="s">
         <v>8</v>
       </c>
@@ -5069,7 +5145,9 @@
       <c r="C91" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D91" s="4"/>
+      <c r="D91" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="G91" s="7"/>
@@ -5084,7 +5162,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="10" t="s">
         <v>8</v>
       </c>
@@ -5094,7 +5172,9 @@
       <c r="C92" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D92" s="4"/>
+      <c r="D92" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
       <c r="G92" s="7"/>
@@ -5109,7 +5189,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="10" t="s">
         <v>8</v>
       </c>
@@ -5119,7 +5199,9 @@
       <c r="C93" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D93" s="4"/>
+      <c r="D93" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="7"/>
@@ -5134,7 +5216,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A94" s="10" t="s">
         <v>8</v>
       </c>
@@ -5144,7 +5226,9 @@
       <c r="C94" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D94" s="4"/>
+      <c r="D94" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="7"/>
@@ -5159,7 +5243,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A95" s="10" t="s">
         <v>8</v>
       </c>
@@ -5169,7 +5253,9 @@
       <c r="C95" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D95" s="4"/>
+      <c r="D95" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
       <c r="G95" s="7"/>
@@ -5184,7 +5270,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="10" t="s">
         <v>8</v>
       </c>
@@ -5194,7 +5280,9 @@
       <c r="C96" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D96" s="4"/>
+      <c r="D96" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
       <c r="G96" s="7"/>
@@ -5209,7 +5297,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
         <v>8</v>
       </c>
@@ -5236,7 +5324,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
         <v>8</v>
       </c>
@@ -5246,7 +5334,9 @@
       <c r="C98" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D98" s="4"/>
+      <c r="D98" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
       <c r="G98" s="7"/>
@@ -5261,7 +5351,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10" t="s">
         <v>8</v>
       </c>
@@ -5271,7 +5361,9 @@
       <c r="C99" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D99" s="4"/>
+      <c r="D99" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
       <c r="G99" s="7"/>
@@ -5286,7 +5378,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="37.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="10" t="s">
         <v>8</v>
       </c>
@@ -5296,7 +5388,9 @@
       <c r="C100" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D100" s="4"/>
+      <c r="D100" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
       <c r="G100" s="7"/>
@@ -5311,7 +5405,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="s">
         <v>8</v>
       </c>
@@ -5320,6 +5414,9 @@
       </c>
       <c r="C101" s="9" t="s">
         <v>137</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -5335,7 +5432,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A102" s="10" t="s">
         <v>8</v>
       </c>
@@ -5362,7 +5459,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A103" s="10" t="s">
         <v>8</v>
       </c>
@@ -5387,7 +5484,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="10" t="s">
         <v>8</v>
       </c>
@@ -5414,7 +5511,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10" t="s">
         <v>8</v>
       </c>
@@ -5424,7 +5521,9 @@
       <c r="C105" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D105" s="6"/>
+      <c r="D105" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
       <c r="G105" s="34"/>
@@ -5439,7 +5538,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="10" t="s">
         <v>8</v>
       </c>
@@ -5449,7 +5548,9 @@
       <c r="C106" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D106" s="6"/>
+      <c r="D106" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
       <c r="G106" s="34"/>
@@ -5464,7 +5565,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="22.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="s">
         <v>8</v>
       </c>
@@ -5474,7 +5575,9 @@
       <c r="C107" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D107" s="6"/>
+      <c r="D107" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
       <c r="G107" s="34"/>
@@ -5489,7 +5592,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A108" s="10" t="s">
         <v>8</v>
       </c>
@@ -5518,7 +5621,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
         <v>8</v>
       </c>
@@ -5545,7 +5648,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A110" s="10" t="s">
         <v>8</v>
       </c>
@@ -5555,7 +5658,9 @@
       <c r="C110" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D110" s="6"/>
+      <c r="D110" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
       <c r="G110" s="34"/>
@@ -5570,7 +5675,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A111" s="10" t="s">
         <v>8</v>
       </c>
@@ -5580,7 +5685,9 @@
       <c r="C111" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D111" s="6"/>
+      <c r="D111" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
       <c r="G111" s="34"/>
@@ -5595,7 +5702,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A112" s="10" t="s">
         <v>8</v>
       </c>
@@ -5622,7 +5729,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A113" s="10" t="s">
         <v>8</v>
       </c>
@@ -5649,7 +5756,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="s">
         <v>8</v>
       </c>
@@ -5676,7 +5783,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="s">
         <v>8</v>
       </c>
@@ -5703,7 +5810,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="10" t="s">
         <v>8</v>
       </c>
@@ -5730,7 +5837,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="10" t="s">
         <v>8</v>
       </c>
@@ -5759,7 +5866,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="118" spans="1:12" s="84" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" s="84" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="78" t="s">
         <v>8</v>
       </c>
@@ -5790,7 +5897,7 @@
         <v>100%</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="10" t="s">
         <v>8</v>
       </c>
@@ -5817,7 +5924,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="10" t="s">
         <v>8</v>
       </c>
@@ -5844,7 +5951,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="10" t="s">
         <v>8</v>
       </c>
@@ -5871,7 +5978,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="122" spans="1:12" s="63" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" s="63" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="64" t="s">
         <v>8</v>
       </c>
@@ -5902,7 +6009,7 @@
         <v>50%</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="31.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="19" t="s">
         <v>8</v>
       </c>
@@ -5912,7 +6019,9 @@
       <c r="C123" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D123" s="4"/>
+      <c r="D123" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
       <c r="H123" s="9"/>
@@ -5925,7 +6034,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A124" s="19" t="s">
         <v>8</v>
       </c>
@@ -5950,7 +6059,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A125" s="19" t="s">
         <v>8</v>
       </c>
@@ -5960,7 +6069,9 @@
       <c r="C125" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D125" s="4"/>
+      <c r="D125" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
       <c r="G125" s="40"/>
@@ -5975,7 +6086,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A126" s="19" t="s">
         <v>8</v>
       </c>
@@ -5985,7 +6096,9 @@
       <c r="C126" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D126" s="4"/>
+      <c r="D126" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
       <c r="G126" s="40"/>
@@ -6000,7 +6113,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A127" s="19" t="s">
         <v>8</v>
       </c>
@@ -6010,7 +6123,9 @@
       <c r="C127" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D127" s="4"/>
+      <c r="D127" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
       <c r="G127" s="40"/>
@@ -6025,7 +6140,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A128" s="19" t="s">
         <v>8</v>
       </c>
@@ -6035,7 +6150,9 @@
       <c r="C128" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="D128" s="6"/>
+      <c r="D128" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E128" s="6"/>
       <c r="F128" s="6"/>
       <c r="G128" s="41"/>
@@ -6050,7 +6167,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A129" s="10" t="s">
         <v>78</v>
       </c>
@@ -6077,7 +6194,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A130" s="10" t="s">
         <v>78</v>
       </c>
@@ -6087,7 +6204,9 @@
       <c r="C130" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D130" s="6"/>
+      <c r="D130" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
       <c r="G130" s="7"/>
@@ -6102,7 +6221,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A131" s="10" t="s">
         <v>78</v>
       </c>
@@ -6129,7 +6248,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A132" s="10" t="s">
         <v>78</v>
       </c>
@@ -6158,7 +6277,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A133" s="10" t="s">
         <v>78</v>
       </c>
@@ -6185,7 +6304,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A134" s="10" t="s">
         <v>78</v>
       </c>
@@ -6212,7 +6331,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A135" s="10" t="s">
         <v>78</v>
       </c>
@@ -6241,7 +6360,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A136" s="10" t="s">
         <v>78</v>
       </c>
@@ -6270,7 +6389,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A137" s="10" t="s">
         <v>78</v>
       </c>
@@ -6297,7 +6416,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A138" s="10" t="s">
         <v>78</v>
       </c>
@@ -6324,7 +6443,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A139" s="10" t="s">
         <v>78</v>
       </c>
@@ -6351,7 +6470,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A140" s="10" t="s">
         <v>78</v>
       </c>
@@ -6378,7 +6497,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A141" s="10" t="s">
         <v>78</v>
       </c>
@@ -6388,7 +6507,9 @@
       <c r="C141" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D141" s="6"/>
+      <c r="D141" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
       <c r="G141" s="36"/>
@@ -6403,7 +6524,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A142" s="10" t="s">
         <v>78</v>
       </c>
@@ -6432,7 +6553,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A143" s="10" t="s">
         <v>78</v>
       </c>
@@ -6459,7 +6580,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" ht="25" x14ac:dyDescent="0.35">
       <c r="A144" s="10" t="s">
         <v>78</v>
       </c>
@@ -6486,7 +6607,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A145" s="10" t="s">
         <v>78</v>
       </c>
@@ -6515,7 +6636,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A146" s="10" t="s">
         <v>78</v>
       </c>
@@ -6544,7 +6665,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A147" s="10" t="s">
         <v>78</v>
       </c>
@@ -6573,7 +6694,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A148" s="10" t="s">
         <v>78</v>
       </c>
@@ -6600,7 +6721,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A149" s="10" t="s">
         <v>78</v>
       </c>
@@ -6625,7 +6746,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A150" s="10" t="s">
         <v>78</v>
       </c>
@@ -6652,7 +6773,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A151" s="10" t="s">
         <v>78</v>
       </c>
@@ -6679,7 +6800,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A152" s="10" t="s">
         <v>78</v>
       </c>
@@ -6706,7 +6827,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A153" s="10" t="s">
         <v>78</v>
       </c>
@@ -6733,7 +6854,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A154" s="10" t="s">
         <v>78</v>
       </c>
@@ -6760,7 +6881,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A155" s="10" t="s">
         <v>78</v>
       </c>
@@ -6787,7 +6908,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A156" s="10" t="s">
         <v>78</v>
       </c>
@@ -6814,7 +6935,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A157" s="10" t="s">
         <v>78</v>
       </c>
@@ -6841,7 +6962,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A158" s="10" t="s">
         <v>78</v>
       </c>
@@ -6868,7 +6989,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A159" s="10" t="s">
         <v>78</v>
       </c>
@@ -6895,7 +7016,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A160" s="85" t="s">
         <v>78</v>
       </c>
@@ -6927,7 +7048,7 @@
       </c>
       <c r="M160" s="93"/>
     </row>
-    <row r="161" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A161" s="10" t="s">
         <v>78</v>
       </c>
@@ -6956,7 +7077,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A162" s="10" t="s">
         <v>78</v>
       </c>
@@ -6966,7 +7087,9 @@
       <c r="C162" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D162" s="6"/>
+      <c r="D162" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E162" s="6"/>
       <c r="F162" s="7"/>
       <c r="G162" s="8"/>
@@ -6981,7 +7104,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A163" s="10" t="s">
         <v>78</v>
       </c>
@@ -6991,7 +7114,9 @@
       <c r="C163" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D163" s="6"/>
+      <c r="D163" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E163" s="6"/>
       <c r="F163" s="7"/>
       <c r="G163" s="8"/>
@@ -7006,7 +7131,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A164" s="10" t="s">
         <v>78</v>
       </c>
@@ -7016,7 +7141,9 @@
       <c r="C164" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D164" s="6"/>
+      <c r="D164" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E164" s="6"/>
       <c r="F164" s="7"/>
       <c r="G164" s="8"/>
@@ -7031,7 +7158,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A165" s="10" t="s">
         <v>78</v>
       </c>
@@ -7041,7 +7168,9 @@
       <c r="C165" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D165" s="6"/>
+      <c r="D165" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E165" s="6"/>
       <c r="F165" s="7"/>
       <c r="G165" s="8"/>
@@ -7056,7 +7185,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A166" s="10" t="s">
         <v>78</v>
       </c>
@@ -7066,7 +7195,9 @@
       <c r="C166" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D166" s="4"/>
+      <c r="D166" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E166" s="4"/>
       <c r="F166" s="4"/>
       <c r="G166" s="7"/>
@@ -7081,7 +7212,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A167" s="78" t="s">
         <v>78</v>
       </c>
@@ -7113,7 +7244,7 @@
       </c>
       <c r="M167" s="84"/>
     </row>
-    <row r="168" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A168" s="10" t="s">
         <v>78</v>
       </c>
@@ -7142,7 +7273,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A169" s="10" t="s">
         <v>78</v>
       </c>
@@ -7171,7 +7302,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A170" s="10" t="s">
         <v>78</v>
       </c>
@@ -7200,7 +7331,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A171" s="10" t="s">
         <v>78</v>
       </c>
@@ -7229,7 +7360,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A172" s="78" t="s">
         <v>78</v>
       </c>
@@ -7261,7 +7392,7 @@
       </c>
       <c r="M172" s="84"/>
     </row>
-    <row r="173" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A173" s="85" t="s">
         <v>78</v>
       </c>
@@ -7293,7 +7424,7 @@
       </c>
       <c r="M173" s="93"/>
     </row>
-    <row r="174" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A174" s="10" t="s">
         <v>78</v>
       </c>
@@ -7320,7 +7451,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A175" s="10" t="s">
         <v>78</v>
       </c>
@@ -7347,7 +7478,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="s">
         <v>78</v>
       </c>
@@ -7374,7 +7505,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A177" s="10" t="s">
         <v>78</v>
       </c>
@@ -7401,7 +7532,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A178" s="10" t="s">
         <v>78</v>
       </c>
@@ -7428,7 +7559,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A179" s="10" t="s">
         <v>78</v>
       </c>
@@ -7455,7 +7586,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A180" s="10" t="s">
         <v>78</v>
       </c>
@@ -7482,7 +7613,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A181" s="10" t="s">
         <v>78</v>
       </c>
@@ -7509,7 +7640,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A182" s="10" t="s">
         <v>78</v>
       </c>
@@ -7536,7 +7667,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="183" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" ht="64.5" x14ac:dyDescent="0.35">
       <c r="A183" s="64" t="s">
         <v>78</v>
       </c>
@@ -7568,14 +7699,16 @@
       </c>
       <c r="M183" s="63"/>
     </row>
-    <row r="184" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A184" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B184" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C184" s="4"/>
+      <c r="C184" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D184" s="4" t="s">
         <v>283</v>
       </c>
@@ -7593,14 +7726,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A185" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B185" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C185" s="4"/>
+      <c r="C185" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D185" s="4" t="s">
         <v>282</v>
       </c>
@@ -7618,14 +7753,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A186" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B186" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C186" s="4"/>
+      <c r="C186" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D186" s="4" t="s">
         <v>277</v>
       </c>
@@ -7643,14 +7780,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A187" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B187" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C187" s="4"/>
+      <c r="C187" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D187" s="4" t="s">
         <v>281</v>
       </c>
@@ -7668,14 +7807,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A188" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B188" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C188" s="4"/>
+      <c r="C188" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D188" s="4" t="s">
         <v>282</v>
       </c>
@@ -7693,14 +7834,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A189" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B189" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C189" s="4"/>
+      <c r="C189" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D189" s="4" t="s">
         <v>283</v>
       </c>
@@ -7718,15 +7861,19 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A190" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B190" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C190" s="4"/>
-      <c r="D190" s="4"/>
+      <c r="C190" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E190" s="4"/>
       <c r="F190" s="4"/>
       <c r="G190" s="7"/>
@@ -7741,14 +7888,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A191" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B191" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C191" s="4"/>
+      <c r="C191" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D191" s="4" t="s">
         <v>283</v>
       </c>
@@ -7766,14 +7915,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A192" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B192" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C192" s="4"/>
+      <c r="C192" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D192" s="4" t="s">
         <v>283</v>
       </c>
@@ -7791,14 +7942,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A193" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B193" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C193" s="4"/>
+      <c r="C193" s="4" t="s">
+        <v>279</v>
+      </c>
       <c r="D193" s="4" t="s">
         <v>283</v>
       </c>
@@ -7816,7 +7969,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A194" s="10" t="s">
         <v>100</v>
       </c>
@@ -7843,14 +7996,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="195" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A195" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B195" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C195" s="5"/>
+      <c r="C195" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D195" s="6" t="s">
         <v>277</v>
       </c>
@@ -7868,14 +8023,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="196" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A196" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C196" s="5"/>
+      <c r="C196" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D196" s="6" t="s">
         <v>277</v>
       </c>
@@ -7893,14 +8050,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A197" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B197" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C197" s="5"/>
+      <c r="C197" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D197" s="6" t="s">
         <v>277</v>
       </c>
@@ -7918,15 +8077,19 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A198" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B198" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C198" s="5"/>
-      <c r="D198" s="6"/>
+      <c r="C198" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D198" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E198" s="6"/>
       <c r="F198" s="6"/>
       <c r="G198" s="7"/>
@@ -7941,14 +8104,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A199" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B199" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C199" s="5"/>
+      <c r="C199" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D199" s="6" t="s">
         <v>277</v>
       </c>
@@ -7966,14 +8131,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A200" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B200" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C200" s="5"/>
+      <c r="C200" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D200" s="6" t="s">
         <v>277</v>
       </c>
@@ -7991,14 +8158,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A201" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B201" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C201" s="5"/>
+      <c r="C201" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D201" s="6" t="s">
         <v>283</v>
       </c>
@@ -8016,14 +8185,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A202" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C202" s="5"/>
+      <c r="C202" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D202" s="6" t="s">
         <v>277</v>
       </c>
@@ -8041,7 +8212,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A203" s="10" t="s">
         <v>100</v>
       </c>
@@ -8069,15 +8240,19 @@
       </c>
       <c r="M203" s="45"/>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A204" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B204" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C204" s="5"/>
-      <c r="D204" s="4"/>
+      <c r="C204" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E204" s="4"/>
       <c r="F204" s="4"/>
       <c r="G204" s="7"/>
@@ -8092,15 +8267,19 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A205" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B205" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C205" s="5"/>
-      <c r="D205" s="4"/>
+      <c r="C205" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E205" s="4"/>
       <c r="F205" s="4"/>
       <c r="G205" s="7"/>
@@ -8115,15 +8294,19 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A206" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B206" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C206" s="5"/>
-      <c r="D206" s="4"/>
+      <c r="C206" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E206" s="4"/>
       <c r="F206" s="4"/>
       <c r="G206" s="7"/>
@@ -8138,7 +8321,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A207" s="10" t="s">
         <v>100</v>
       </c>
@@ -8148,7 +8331,9 @@
       <c r="C207" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D207" s="6"/>
+      <c r="D207" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="E207" s="6"/>
       <c r="F207" s="4"/>
       <c r="G207" s="7"/>
@@ -8163,7 +8348,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A208" s="64" t="s">
         <v>100</v>
       </c>
@@ -8193,7 +8378,7 @@
       </c>
       <c r="M208" s="63"/>
     </row>
-    <row r="209" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A209" s="64" t="s">
         <v>100</v>
       </c>
@@ -8223,7 +8408,7 @@
       </c>
       <c r="M209" s="63"/>
     </row>
-    <row r="210" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A210" s="64" t="s">
         <v>100</v>
       </c>
@@ -8253,7 +8438,7 @@
       </c>
       <c r="M210" s="63"/>
     </row>
-    <row r="211" spans="1:13" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A211" s="64" t="s">
         <v>100</v>
       </c>
@@ -8283,12 +8468,14 @@
       </c>
       <c r="M211" s="63"/>
     </row>
-    <row r="212" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A212" s="64" t="s">
         <v>100</v>
       </c>
       <c r="B212" s="66"/>
-      <c r="C212" s="77"/>
+      <c r="C212" s="77" t="s">
+        <v>279</v>
+      </c>
       <c r="D212" s="66" t="s">
         <v>282</v>
       </c>
@@ -8309,12 +8496,14 @@
       </c>
       <c r="M212" s="63"/>
     </row>
-    <row r="213" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A213" s="64" t="s">
         <v>100</v>
       </c>
       <c r="B213" s="66"/>
-      <c r="C213" s="77"/>
+      <c r="C213" s="77" t="s">
+        <v>279</v>
+      </c>
       <c r="D213" s="66" t="s">
         <v>281</v>
       </c>
@@ -8335,12 +8524,14 @@
       </c>
       <c r="M213" s="63"/>
     </row>
-    <row r="214" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A214" s="64" t="s">
         <v>100</v>
       </c>
       <c r="B214" s="66"/>
-      <c r="C214" s="77"/>
+      <c r="C214" s="77" t="s">
+        <v>279</v>
+      </c>
       <c r="D214" s="66" t="s">
         <v>277</v>
       </c>
@@ -8361,12 +8552,14 @@
       </c>
       <c r="M214" s="63"/>
     </row>
-    <row r="215" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A215" s="64" t="s">
         <v>100</v>
       </c>
       <c r="B215" s="66"/>
-      <c r="C215" s="77"/>
+      <c r="C215" s="77" t="s">
+        <v>279</v>
+      </c>
       <c r="D215" s="66" t="s">
         <v>283</v>
       </c>
@@ -8387,7 +8580,7 @@
       </c>
       <c r="M215" s="63"/>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A216" s="10" t="s">
         <v>100</v>
       </c>
@@ -8416,7 +8609,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A217" s="10" t="s">
         <v>100</v>
       </c>
@@ -8445,7 +8638,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A218" s="10" t="s">
         <v>100</v>
       </c>
@@ -8474,7 +8667,7 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A219" s="10" t="s">
         <v>100</v>
       </c>
@@ -8503,14 +8696,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="25" x14ac:dyDescent="0.35">
       <c r="A220" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B220" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C220" s="5"/>
+      <c r="C220" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D220" s="6" t="s">
         <v>277</v>
       </c>
@@ -8528,14 +8723,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" ht="13" x14ac:dyDescent="0.35">
       <c r="A221" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B221" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C221" s="5"/>
+      <c r="C221" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="D221" s="4" t="s">
         <v>282</v>
       </c>
@@ -8553,15 +8750,19 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" ht="13" x14ac:dyDescent="0.35">
       <c r="A222" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B222" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C222" s="4"/>
-      <c r="D222" s="4"/>
+      <c r="C222" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="E222" s="98" t="s">
         <v>245</v>
       </c>
@@ -8578,14 +8779,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A223" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B223" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C223" s="7"/>
+      <c r="C223" s="7" t="s">
+        <v>279</v>
+      </c>
       <c r="D223" s="7" t="s">
         <v>283</v>
       </c>
@@ -8605,14 +8808,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="224" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A224" s="84" t="s">
         <v>100</v>
       </c>
       <c r="B224" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C224" s="82"/>
+      <c r="C224" s="82" t="s">
+        <v>279</v>
+      </c>
       <c r="D224" s="82" t="s">
         <v>281</v>
       </c>
@@ -8633,14 +8838,16 @@
       </c>
       <c r="M224" s="84"/>
     </row>
-    <row r="225" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" ht="39" x14ac:dyDescent="0.35">
       <c r="A225" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B225" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C225" s="7"/>
+      <c r="C225" s="7" t="s">
+        <v>279</v>
+      </c>
       <c r="D225" s="7" t="s">
         <v>277</v>
       </c>
@@ -8660,14 +8867,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="226" spans="1:13" ht="51" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" ht="51.5" x14ac:dyDescent="0.35">
       <c r="A226" s="84" t="s">
         <v>100</v>
       </c>
       <c r="B226" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C226" s="82"/>
+      <c r="C226" s="82" t="s">
+        <v>279</v>
+      </c>
       <c r="D226" s="82" t="s">
         <v>283</v>
       </c>
@@ -8688,14 +8897,16 @@
       </c>
       <c r="M226" s="84"/>
     </row>
-    <row r="227" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A227" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B227" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C227" s="7"/>
+      <c r="C227" s="7" t="s">
+        <v>279</v>
+      </c>
       <c r="D227" s="7" t="s">
         <v>282</v>
       </c>
@@ -8715,14 +8926,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="228" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A228" s="84" t="s">
         <v>100</v>
       </c>
       <c r="B228" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C228" s="82"/>
+      <c r="C228" s="82" t="s">
+        <v>279</v>
+      </c>
       <c r="D228" s="82" t="s">
         <v>281</v>
       </c>
@@ -8743,15 +8956,19 @@
       </c>
       <c r="M228" s="84"/>
     </row>
-    <row r="229" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A229" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B229" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C229" s="7"/>
-      <c r="D229" s="7"/>
+      <c r="C229" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D229" s="7" t="s">
+        <v>285</v>
+      </c>
       <c r="E229" s="99" t="s">
         <v>254</v>
       </c>
@@ -8768,14 +8985,16 @@
         <v>30%</v>
       </c>
     </row>
-    <row r="230" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A230" s="84" t="s">
         <v>100</v>
       </c>
       <c r="B230" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C230" s="82"/>
+      <c r="C230" s="82" t="s">
+        <v>279</v>
+      </c>
       <c r="D230" s="82" t="s">
         <v>281</v>
       </c>
@@ -8796,14 +9015,16 @@
       </c>
       <c r="M230" s="84"/>
     </row>
-    <row r="231" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A231" s="84" t="s">
         <v>100</v>
       </c>
       <c r="B231" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C231" s="82"/>
+      <c r="C231" s="82" t="s">
+        <v>279</v>
+      </c>
       <c r="D231" s="82" t="s">
         <v>283</v>
       </c>
@@ -8825,7 +9046,6 @@
       <c r="M231" s="84"/>
     </row>
   </sheetData>
-  <autoFilter ref="C2:C7" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="I71:I73">
     <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(I71,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(I71,0)&lt;(WEEKDAY(TODAY())+7))</formula>
@@ -8864,29 +9084,29 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -8904,16 +9124,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="47" customWidth="1"/>
-    <col min="2" max="2" width="56.85546875" style="47" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="47" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="47"/>
+    <col min="2" max="2" width="56.81640625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" style="47" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="111" t="s">
         <v>238</v>
       </c>
@@ -8921,7 +9141,7 @@
       <c r="C1" s="111"/>
       <c r="D1" s="111"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
         <v>235</v>
       </c>
@@ -8935,7 +9155,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>116</v>
       </c>
@@ -8949,7 +9169,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>116</v>
       </c>
@@ -8963,7 +9183,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
         <v>116</v>
       </c>
@@ -8977,7 +9197,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
         <v>116</v>
       </c>
@@ -8991,7 +9211,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
         <v>116</v>
       </c>
@@ -9005,7 +9225,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
         <v>116</v>
       </c>
@@ -9019,7 +9239,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>116</v>
       </c>
@@ -9033,7 +9253,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="25" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
         <v>139</v>
       </c>
@@ -9047,7 +9267,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>227</v>
       </c>
@@ -9057,7 +9277,7 @@
       <c r="C11" s="51"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
         <v>219</v>
@@ -9071,7 +9291,7 @@
       <c r="H12" s="19"/>
       <c r="J12" s="19"/>
     </row>
-    <row r="13" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
         <v>222</v>
@@ -9085,7 +9305,7 @@
       <c r="H13" s="19"/>
       <c r="J13" s="19"/>
     </row>
-    <row r="14" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
         <v>221</v>
@@ -9099,7 +9319,7 @@
       <c r="H14" s="19"/>
       <c r="J14" s="19"/>
     </row>
-    <row r="15" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
         <v>224</v>
@@ -9113,7 +9333,7 @@
       <c r="H15" s="19"/>
       <c r="J15" s="19"/>
     </row>
-    <row r="16" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
         <v>223</v>
@@ -9127,7 +9347,7 @@
       <c r="H16" s="19"/>
       <c r="J16" s="19"/>
     </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
         <v>225</v>
@@ -9141,7 +9361,7 @@
       <c r="H17" s="19"/>
       <c r="J17" s="19"/>
     </row>
-    <row r="18" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="9" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
         <v>220</v>
@@ -9155,7 +9375,7 @@
       <c r="H18" s="19"/>
       <c r="J18" s="19"/>
     </row>
-    <row r="19" spans="1:10" s="53" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="53" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
         <v>116</v>
       </c>
@@ -9167,7 +9387,7 @@
       </c>
       <c r="D19" s="55"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="51"/>
       <c r="B20" s="51" t="s">
         <v>242</v>
@@ -9194,14 +9414,14 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="56" t="s">
         <v>247</v>
       </c>

</xml_diff>

<commit_message>
deletion in sections not working
</commit_message>
<xml_diff>
--- a/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
+++ b/dashboard/online_help/management/dataset/Radiant_2025.1_help_assignments_v3_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latticesemiconductor4-my.sharepoint.com/personal/jonathan_bunquin_latticesemi_com/Documents/Documents/GitHub/help_dashboard_django/dashboard/online_help/management/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="646" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BD08390-BC7E-4E2C-A7AA-4290D8184169}"/>
+  <xr:revisionPtr revIDLastSave="721" documentId="13_ncr:1_{F0CE50B6-F27D-4933-933C-D230C28C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDCE931E-27DA-4850-AE26-905D75238A9D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="ECNs" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025.1'!$A$1:$M$231</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025.1'!$A$1:$M$228</definedName>
     <definedName name="_Hlk95147257" localSheetId="0">'2025.1'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="285">
   <si>
     <t>Radiant Documentation</t>
   </si>
@@ -801,9 +801,6 @@
   </si>
   <si>
     <t xml:space="preserve">MachXO4D </t>
-  </si>
-  <si>
-    <t>ERD-03.08 DNG-22303 Mach-XO4 Support (Phase 1) ERD - Partial for EAPR</t>
   </si>
   <si>
     <t>PARTIAL</t>
@@ -1051,22 +1048,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">ERD-09.06 Support post par reveal flow
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>05/13/2025 -- Done. Added content provided by Pradeep: User Guides &gt; Testing and Debugging On-Chip &gt; About Reveal Logic Analysis &gt; Post-PAR Reveal Incremental Flow
-Sent for review</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>•</t>
     </r>
     <r>
@@ -1570,6 +1551,23 @@
   <si>
     <t>no writer</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ERD-09.06 Support post par reveal flow
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>05/13/2025 -- Done. Added content provided by Pradeep: User Guides &gt; Testing and Debugging On-Chip &gt; About Reveal Logic Analysis &gt; Post-PAR Reve
+ERD-03.08 DNG-22303 Mach-XO4 Support (Phase 1) ERD - Partial for EAPRal Incremental Flow
+Sent for review</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1578,7 +1576,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1689,13 +1687,6 @@
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1922,7 +1913,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2206,12 +2197,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2618,11 +2603,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M231"/>
+  <dimension ref="A1:M228"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C237" sqref="C237"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -2642,7 +2627,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="102.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
@@ -2654,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>130</v>
@@ -2672,29 +2657,29 @@
         <v>7</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="63" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="103" t="s">
-        <v>277</v>
-      </c>
-      <c r="E2" s="104" t="s">
+      <c r="D2" s="101" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="102" t="s">
         <v>212</v>
       </c>
       <c r="F2" s="58"/>
@@ -2703,7 +2688,7 @@
       <c r="I2" s="61"/>
       <c r="J2" s="62"/>
       <c r="K2" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L2" s="9" t="str">
         <f>IF(K2="Yellow", "50%", IF(K2="Green", "100%", IF(K2="Grey", "0%", IF(K2="White", "30%", IF(K2="Orange", "10%", "")))))</f>
@@ -2714,16 +2699,16 @@
       <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="103" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="103" t="s">
-        <v>277</v>
-      </c>
-      <c r="E3" s="106" t="s">
+      <c r="D3" s="101" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="104" t="s">
         <v>213</v>
       </c>
       <c r="F3" s="60"/>
@@ -2732,7 +2717,7 @@
       <c r="I3" s="61"/>
       <c r="J3" s="62"/>
       <c r="K3" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L3" s="9" t="str">
         <f t="shared" ref="L3:L66" si="0">IF(K3="Yellow", "50%", IF(K3="Green", "100%", IF(K3="Grey", "0%", IF(K3="White", "30%", IF(K3="Orange", "10%", "")))))</f>
@@ -2743,16 +2728,16 @@
       <c r="A4" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="103" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="103" t="s">
-        <v>277</v>
-      </c>
-      <c r="E4" s="106" t="s">
+      <c r="D4" s="101" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="104" t="s">
         <v>213</v>
       </c>
       <c r="F4" s="60"/>
@@ -2761,7 +2746,7 @@
       <c r="I4" s="61"/>
       <c r="J4" s="62"/>
       <c r="K4" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L4" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2779,7 +2764,7 @@
         <v>142</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -2788,7 +2773,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="8"/>
       <c r="K5" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L5" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2806,7 +2791,7 @@
         <v>143</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -2815,7 +2800,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="8"/>
       <c r="K6" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L6" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2829,11 +2814,11 @@
       <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="108" t="s">
         <v>144</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -2842,7 +2827,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="8"/>
       <c r="K7" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L7" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2860,7 +2845,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2869,7 +2854,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="8"/>
       <c r="K8" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L8" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2887,7 +2872,7 @@
         <v>145</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2896,7 +2881,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="8"/>
       <c r="K9" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L9" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2914,7 +2899,7 @@
         <v>146</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -2923,7 +2908,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="8"/>
       <c r="K10" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L10" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2941,7 +2926,7 @@
         <v>147</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -2950,7 +2935,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
       <c r="K11" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L11" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2968,7 +2953,7 @@
         <v>148</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -2977,7 +2962,7 @@
       <c r="I12" s="7"/>
       <c r="J12" s="8"/>
       <c r="K12" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L12" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2995,7 +2980,7 @@
         <v>149</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -3004,7 +2989,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="8"/>
       <c r="K13" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L13" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3022,7 +3007,7 @@
         <v>150</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -3031,7 +3016,7 @@
       <c r="I14" s="7"/>
       <c r="J14" s="8"/>
       <c r="K14" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L14" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3049,7 +3034,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -3058,7 +3043,7 @@
       <c r="I15" s="7"/>
       <c r="J15" s="8"/>
       <c r="K15" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L15" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3076,7 +3061,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -3085,7 +3070,7 @@
       <c r="I16" s="7"/>
       <c r="J16" s="8"/>
       <c r="K16" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L16" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3103,7 +3088,7 @@
         <v>151</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -3112,7 +3097,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="8"/>
       <c r="K17" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L17" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3130,7 +3115,7 @@
         <v>14</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -3139,7 +3124,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="8"/>
       <c r="K18" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L18" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3157,7 +3142,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -3166,7 +3151,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="8"/>
       <c r="K19" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L19" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3184,7 +3169,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -3193,7 +3178,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="8"/>
       <c r="K20" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L20" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3211,7 +3196,7 @@
         <v>152</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -3220,7 +3205,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="8"/>
       <c r="K21" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L21" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3238,7 +3223,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -3247,7 +3232,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="8"/>
       <c r="K22" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L22" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3265,7 +3250,7 @@
         <v>153</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -3274,7 +3259,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="8"/>
       <c r="K23" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L23" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3288,16 +3273,16 @@
       <c r="B24" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="107" t="s">
+      <c r="C24" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="108" t="s">
-        <v>282</v>
-      </c>
-      <c r="E24" s="108" t="s">
-        <v>261</v>
-      </c>
-      <c r="F24" s="108" t="s">
+      <c r="D24" s="106" t="s">
+        <v>280</v>
+      </c>
+      <c r="E24" s="106" t="s">
+        <v>259</v>
+      </c>
+      <c r="F24" s="106" t="s">
         <v>214</v>
       </c>
       <c r="G24" s="82"/>
@@ -3305,7 +3290,7 @@
       <c r="I24" s="82"/>
       <c r="J24" s="83"/>
       <c r="K24" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L24" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3319,16 +3304,16 @@
       <c r="B25" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="107" t="s">
+      <c r="C25" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="108" t="s">
-        <v>283</v>
-      </c>
-      <c r="E25" s="108" t="s">
-        <v>261</v>
-      </c>
-      <c r="F25" s="108" t="s">
+      <c r="D25" s="106" t="s">
+        <v>281</v>
+      </c>
+      <c r="E25" s="106" t="s">
+        <v>259</v>
+      </c>
+      <c r="F25" s="106" t="s">
         <v>214</v>
       </c>
       <c r="G25" s="82"/>
@@ -3336,7 +3321,7 @@
       <c r="I25" s="82"/>
       <c r="J25" s="83"/>
       <c r="K25" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L25" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3354,7 +3339,7 @@
         <v>154</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -3363,7 +3348,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="8"/>
       <c r="K26" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L26" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3381,7 +3366,7 @@
         <v>11</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -3390,7 +3375,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="8"/>
       <c r="K27" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L27" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3408,7 +3393,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -3417,7 +3402,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="8"/>
       <c r="K28" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L28" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3435,7 +3420,7 @@
         <v>155</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -3444,7 +3429,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="8"/>
       <c r="K29" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L29" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3462,7 +3447,7 @@
         <v>20</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -3471,7 +3456,7 @@
       <c r="I30" s="7"/>
       <c r="J30" s="4"/>
       <c r="K30" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L30" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3489,7 +3474,7 @@
         <v>21</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
@@ -3500,7 +3485,7 @@
       <c r="I31" s="7"/>
       <c r="J31" s="4"/>
       <c r="K31" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L31" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3518,7 +3503,7 @@
         <v>11</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -3527,7 +3512,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L32" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3545,7 +3530,7 @@
         <v>156</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -3554,7 +3539,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L33" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3572,7 +3557,7 @@
         <v>157</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -3581,7 +3566,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L34" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3599,7 +3584,7 @@
         <v>158</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -3608,7 +3593,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L35" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3626,7 +3611,7 @@
         <v>159</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
@@ -3637,7 +3622,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L36" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3655,7 +3640,7 @@
         <v>160</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="4" t="s">
@@ -3666,7 +3651,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L37" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3684,7 +3669,7 @@
         <v>11</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
@@ -3693,7 +3678,7 @@
       <c r="I38" s="25"/>
       <c r="J38" s="26"/>
       <c r="K38" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L38" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3711,7 +3696,7 @@
         <v>161</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
@@ -3722,7 +3707,7 @@
       <c r="I39" s="13"/>
       <c r="J39" s="8"/>
       <c r="K39" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L39" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3740,7 +3725,7 @@
         <v>24</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -3749,7 +3734,7 @@
       <c r="I40" s="13"/>
       <c r="J40" s="8"/>
       <c r="K40" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L40" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3767,7 +3752,7 @@
         <v>25</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -3776,7 +3761,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="8"/>
       <c r="K41" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L41" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3794,7 +3779,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="7"/>
@@ -3803,7 +3788,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="8"/>
       <c r="K42" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L42" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3821,7 +3806,7 @@
         <v>119</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -3830,7 +3815,7 @@
       <c r="I43" s="7"/>
       <c r="J43" s="8"/>
       <c r="K43" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L43" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3848,7 +3833,7 @@
         <v>27</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -3857,7 +3842,7 @@
       <c r="I44" s="7"/>
       <c r="J44" s="8"/>
       <c r="K44" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L44" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3875,7 +3860,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -3884,7 +3869,7 @@
       <c r="I45" s="7"/>
       <c r="J45" s="8"/>
       <c r="K45" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L45" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3902,7 +3887,7 @@
         <v>28</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -3911,7 +3896,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L46" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3929,7 +3914,7 @@
         <v>163</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E47" s="28"/>
       <c r="F47" s="28"/>
@@ -3938,7 +3923,7 @@
       <c r="I47" s="29"/>
       <c r="J47" s="28"/>
       <c r="K47" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L47" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3956,7 +3941,7 @@
         <v>164</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E48" s="28"/>
       <c r="F48" s="28"/>
@@ -3965,7 +3950,7 @@
       <c r="I48" s="29"/>
       <c r="J48" s="28"/>
       <c r="K48" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L48" s="9" t="str">
         <f t="shared" si="0"/>
@@ -3983,7 +3968,7 @@
         <v>165</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E49" s="28"/>
       <c r="F49" s="28"/>
@@ -3992,7 +3977,7 @@
       <c r="I49" s="29"/>
       <c r="J49" s="28"/>
       <c r="K49" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L49" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4010,7 +3995,7 @@
         <v>120</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E50" s="28"/>
       <c r="F50" s="28"/>
@@ -4019,7 +4004,7 @@
       <c r="I50" s="29"/>
       <c r="J50" s="28"/>
       <c r="K50" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L50" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4037,10 +4022,10 @@
         <v>166</v>
       </c>
       <c r="D51" s="60" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E51" s="58" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F51" s="70" t="s">
         <v>216</v>
@@ -4050,7 +4035,7 @@
       <c r="I51" s="71"/>
       <c r="J51" s="70"/>
       <c r="K51" s="72" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L51" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4068,10 +4053,10 @@
         <v>166</v>
       </c>
       <c r="D52" s="60" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E52" s="58" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F52" s="70" t="s">
         <v>216</v>
@@ -4081,7 +4066,7 @@
       <c r="I52" s="71"/>
       <c r="J52" s="70"/>
       <c r="K52" s="72" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L52" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4099,10 +4084,10 @@
         <v>166</v>
       </c>
       <c r="D53" s="60" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E53" s="58" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F53" s="70" t="s">
         <v>216</v>
@@ -4112,7 +4097,7 @@
       <c r="I53" s="71"/>
       <c r="J53" s="70"/>
       <c r="K53" s="72" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L53" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4130,7 +4115,7 @@
         <v>29</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -4139,7 +4124,7 @@
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
       <c r="K54" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L54" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4157,10 +4142,10 @@
         <v>30</v>
       </c>
       <c r="D55" s="81" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E55" s="81" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F55" s="81"/>
       <c r="G55" s="82"/>
@@ -4168,7 +4153,7 @@
       <c r="I55" s="82"/>
       <c r="J55" s="83"/>
       <c r="K55" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L55" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4186,7 +4171,7 @@
         <v>167</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -4195,7 +4180,7 @@
       <c r="I56" s="7"/>
       <c r="J56" s="8"/>
       <c r="K56" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L56" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4213,7 +4198,7 @@
         <v>31</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -4222,7 +4207,7 @@
       <c r="I57" s="7"/>
       <c r="J57" s="8"/>
       <c r="K57" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L57" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4240,7 +4225,7 @@
         <v>168</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -4249,7 +4234,7 @@
       <c r="I58" s="7"/>
       <c r="J58" s="8"/>
       <c r="K58" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L58" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4267,7 +4252,7 @@
         <v>169</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -4276,7 +4261,7 @@
       <c r="I59" s="7"/>
       <c r="J59" s="8"/>
       <c r="K59" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L59" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4294,7 +4279,7 @@
         <v>11</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -4303,7 +4288,7 @@
       <c r="I60" s="13"/>
       <c r="J60" s="8"/>
       <c r="K60" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L60" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4321,7 +4306,7 @@
         <v>33</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -4330,7 +4315,7 @@
       <c r="I61" s="13"/>
       <c r="J61" s="8"/>
       <c r="K61" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L61" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4348,7 +4333,7 @@
         <v>34</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="7"/>
@@ -4356,7 +4341,7 @@
       <c r="I62" s="13"/>
       <c r="J62" s="8"/>
       <c r="K62" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L62" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4374,7 +4359,7 @@
         <v>35</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -4383,7 +4368,7 @@
       <c r="I63" s="13"/>
       <c r="J63" s="8"/>
       <c r="K63" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L63" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4401,7 +4386,7 @@
         <v>36</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -4410,7 +4395,7 @@
       <c r="I64" s="13"/>
       <c r="J64" s="8"/>
       <c r="K64" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L64" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4425,10 +4410,10 @@
         <v>32</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -4437,7 +4422,7 @@
       <c r="I65" s="13"/>
       <c r="J65" s="8"/>
       <c r="K65" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L65" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4455,7 +4440,7 @@
         <v>117</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -4464,7 +4449,7 @@
       <c r="I66" s="13"/>
       <c r="J66" s="8"/>
       <c r="K66" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L66" s="9" t="str">
         <f t="shared" si="0"/>
@@ -4482,7 +4467,7 @@
         <v>203</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E67" s="19"/>
       <c r="F67" s="18"/>
@@ -4491,7 +4476,7 @@
       <c r="I67" s="25"/>
       <c r="J67" s="26"/>
       <c r="K67" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L67" s="9" t="str">
         <f t="shared" ref="L67:L130" si="1">IF(K67="Yellow", "50%", IF(K67="Green", "100%", IF(K67="Grey", "0%", IF(K67="White", "30%", IF(K67="Orange", "10%", "")))))</f>
@@ -4509,7 +4494,7 @@
         <v>11</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E68" s="7"/>
       <c r="F68" s="18"/>
@@ -4518,7 +4503,7 @@
       <c r="I68" s="25"/>
       <c r="J68" s="26"/>
       <c r="K68" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L68" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4536,7 +4521,7 @@
         <v>121</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="18"/>
@@ -4545,7 +4530,7 @@
       <c r="I69" s="24"/>
       <c r="J69" s="26"/>
       <c r="K69" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L69" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4563,7 +4548,7 @@
         <v>122</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="18"/>
@@ -4572,7 +4557,7 @@
       <c r="I70" s="7"/>
       <c r="J70" s="8"/>
       <c r="K70" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L70" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4590,7 +4575,7 @@
         <v>170</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E71" s="18"/>
       <c r="F71" s="18"/>
@@ -4599,7 +4584,7 @@
       <c r="I71" s="8"/>
       <c r="J71" s="8"/>
       <c r="K71" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L71" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4617,7 +4602,7 @@
         <v>133</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="18" t="s">
@@ -4628,7 +4613,7 @@
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
       <c r="K72" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L72" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4646,7 +4631,7 @@
         <v>133</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="18" t="s">
@@ -4657,7 +4642,7 @@
       <c r="I73" s="8"/>
       <c r="J73" s="8"/>
       <c r="K73" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L73" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4675,7 +4660,7 @@
         <v>125</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
@@ -4684,7 +4669,7 @@
       <c r="I74" s="7"/>
       <c r="J74" s="8"/>
       <c r="K74" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L74" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4702,7 +4687,7 @@
         <v>11</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -4711,7 +4696,7 @@
       <c r="I75" s="7"/>
       <c r="J75" s="8"/>
       <c r="K75" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L75" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4729,7 +4714,7 @@
         <v>39</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -4738,7 +4723,7 @@
       <c r="I76" s="7"/>
       <c r="J76" s="8"/>
       <c r="K76" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L76" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4756,7 +4741,7 @@
         <v>40</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -4765,7 +4750,7 @@
       <c r="I77" s="7"/>
       <c r="J77" s="8"/>
       <c r="K77" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L77" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4783,7 +4768,7 @@
         <v>41</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -4792,7 +4777,7 @@
       <c r="I78" s="7"/>
       <c r="J78" s="8"/>
       <c r="K78" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L78" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4810,7 +4795,7 @@
         <v>42</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -4819,7 +4804,7 @@
       <c r="I79" s="7"/>
       <c r="J79" s="8"/>
       <c r="K79" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L79" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4837,7 +4822,7 @@
         <v>43</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
@@ -4846,7 +4831,7 @@
       <c r="I80" s="7"/>
       <c r="J80" s="8"/>
       <c r="K80" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L80" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4864,7 +4849,7 @@
         <v>44</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
@@ -4873,7 +4858,7 @@
       <c r="I81" s="7"/>
       <c r="J81" s="8"/>
       <c r="K81" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L81" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4891,7 +4876,7 @@
         <v>45</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
@@ -4900,7 +4885,7 @@
       <c r="I82" s="7"/>
       <c r="J82" s="8"/>
       <c r="K82" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L82" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4918,7 +4903,7 @@
         <v>46</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
@@ -4927,7 +4912,7 @@
       <c r="I83" s="7"/>
       <c r="J83" s="8"/>
       <c r="K83" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L83" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4945,7 +4930,7 @@
         <v>171</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -4954,7 +4939,7 @@
       <c r="I84" s="7"/>
       <c r="J84" s="8"/>
       <c r="K84" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L84" s="9" t="str">
         <f t="shared" si="1"/>
@@ -4972,20 +4957,20 @@
         <v>47</v>
       </c>
       <c r="D85" s="58" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E85" s="94" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F85" s="58" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G85" s="61"/>
       <c r="H85" s="61"/>
       <c r="I85" s="62"/>
       <c r="J85" s="62"/>
       <c r="K85" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L85" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5003,7 +4988,7 @@
         <v>48</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -5012,7 +4997,7 @@
       <c r="I86" s="7"/>
       <c r="J86" s="8"/>
       <c r="K86" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L86" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5030,20 +5015,20 @@
         <v>49</v>
       </c>
       <c r="D87" s="58" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E87" s="58" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F87" s="74" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G87" s="61"/>
       <c r="H87" s="61"/>
       <c r="I87" s="61"/>
       <c r="J87" s="62"/>
       <c r="K87" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L87" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5061,20 +5046,20 @@
         <v>49</v>
       </c>
       <c r="D88" s="58" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E88" s="58" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F88" s="74" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G88" s="61"/>
       <c r="H88" s="61"/>
       <c r="I88" s="61"/>
       <c r="J88" s="62"/>
       <c r="K88" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L88" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5092,7 +5077,7 @@
         <v>50</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -5101,7 +5086,7 @@
       <c r="I89" s="8"/>
       <c r="J89" s="8"/>
       <c r="K89" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L89" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5119,7 +5104,7 @@
         <v>51</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
@@ -5128,7 +5113,7 @@
       <c r="I90" s="7"/>
       <c r="J90" s="8"/>
       <c r="K90" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L90" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5146,7 +5131,7 @@
         <v>52</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
@@ -5155,7 +5140,7 @@
       <c r="I91" s="7"/>
       <c r="J91" s="8"/>
       <c r="K91" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L91" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5173,7 +5158,7 @@
         <v>53</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -5182,7 +5167,7 @@
       <c r="I92" s="7"/>
       <c r="J92" s="8"/>
       <c r="K92" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L92" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5200,7 +5185,7 @@
         <v>54</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
@@ -5209,7 +5194,7 @@
       <c r="I93" s="7"/>
       <c r="J93" s="8"/>
       <c r="K93" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L93" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5227,7 +5212,7 @@
         <v>55</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
@@ -5236,7 +5221,7 @@
       <c r="I94" s="7"/>
       <c r="J94" s="8"/>
       <c r="K94" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L94" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5254,7 +5239,7 @@
         <v>56</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
@@ -5263,7 +5248,7 @@
       <c r="I95" s="7"/>
       <c r="J95" s="8"/>
       <c r="K95" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L95" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5281,7 +5266,7 @@
         <v>118</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
@@ -5290,7 +5275,7 @@
       <c r="I96" s="7"/>
       <c r="J96" s="8"/>
       <c r="K96" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L96" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5308,7 +5293,7 @@
         <v>57</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
@@ -5317,7 +5302,7 @@
       <c r="I97" s="7"/>
       <c r="J97" s="8"/>
       <c r="K97" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L97" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5335,7 +5320,7 @@
         <v>58</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
@@ -5344,7 +5329,7 @@
       <c r="I98" s="7"/>
       <c r="J98" s="8"/>
       <c r="K98" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L98" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5362,7 +5347,7 @@
         <v>59</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
@@ -5371,7 +5356,7 @@
       <c r="I99" s="7"/>
       <c r="J99" s="8"/>
       <c r="K99" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L99" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5389,7 +5374,7 @@
         <v>60</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4"/>
@@ -5398,7 +5383,7 @@
       <c r="I100" s="7"/>
       <c r="J100" s="8"/>
       <c r="K100" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L100" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5416,7 +5401,7 @@
         <v>137</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
@@ -5425,7 +5410,7 @@
       <c r="I101" s="7"/>
       <c r="J101" s="8"/>
       <c r="K101" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L101" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5443,7 +5428,7 @@
         <v>11</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
@@ -5452,7 +5437,7 @@
       <c r="I102" s="31"/>
       <c r="J102" s="8"/>
       <c r="K102" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L102" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5468,7 +5453,7 @@
         <v>62</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E103" s="6"/>
       <c r="F103" s="4"/>
@@ -5477,7 +5462,7 @@
       <c r="I103" s="32"/>
       <c r="J103" s="8"/>
       <c r="K103" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L103" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5495,7 +5480,7 @@
         <v>11</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -5504,7 +5489,7 @@
       <c r="I104" s="33"/>
       <c r="J104" s="33"/>
       <c r="K104" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L104" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5522,7 +5507,7 @@
         <v>172</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -5531,7 +5516,7 @@
       <c r="I105" s="34"/>
       <c r="J105" s="34"/>
       <c r="K105" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L105" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5549,7 +5534,7 @@
         <v>173</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
@@ -5558,7 +5543,7 @@
       <c r="I106" s="34"/>
       <c r="J106" s="34"/>
       <c r="K106" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L106" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5576,7 +5561,7 @@
         <v>174</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
@@ -5585,7 +5570,7 @@
       <c r="I107" s="34"/>
       <c r="J107" s="34"/>
       <c r="K107" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L107" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5603,7 +5588,7 @@
         <v>175</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4" t="s">
@@ -5614,7 +5599,7 @@
       <c r="I108" s="34"/>
       <c r="J108" s="34"/>
       <c r="K108" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L108" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5632,7 +5617,7 @@
         <v>64</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
@@ -5641,7 +5626,7 @@
       <c r="I109" s="34"/>
       <c r="J109" s="34"/>
       <c r="K109" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L109" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5659,7 +5644,7 @@
         <v>176</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
@@ -5668,7 +5653,7 @@
       <c r="I110" s="34"/>
       <c r="J110" s="34"/>
       <c r="K110" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L110" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5686,7 +5671,7 @@
         <v>177</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
@@ -5695,7 +5680,7 @@
       <c r="I111" s="34"/>
       <c r="J111" s="34"/>
       <c r="K111" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L111" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5713,7 +5698,7 @@
         <v>65</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
@@ -5722,7 +5707,7 @@
       <c r="I112" s="34"/>
       <c r="J112" s="34"/>
       <c r="K112" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L112" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5740,7 +5725,7 @@
         <v>66</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
@@ -5749,7 +5734,7 @@
       <c r="I113" s="34"/>
       <c r="J113" s="34"/>
       <c r="K113" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L113" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5767,7 +5752,7 @@
         <v>67</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -5776,7 +5761,7 @@
       <c r="I114" s="34"/>
       <c r="J114" s="34"/>
       <c r="K114" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L114" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5794,7 +5779,7 @@
         <v>68</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
@@ -5803,7 +5788,7 @@
       <c r="I115" s="34"/>
       <c r="J115" s="34"/>
       <c r="K115" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L115" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5821,7 +5806,7 @@
         <v>69</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -5830,7 +5815,7 @@
       <c r="I116" s="34"/>
       <c r="J116" s="34"/>
       <c r="K116" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L116" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5848,7 +5833,7 @@
         <v>11</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E117" s="4"/>
       <c r="F117" s="4" t="s">
@@ -5859,7 +5844,7 @@
       <c r="I117" s="7"/>
       <c r="J117" s="8"/>
       <c r="K117" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L117" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5877,10 +5862,10 @@
         <v>71</v>
       </c>
       <c r="D118" s="81" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E118" s="81" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F118" s="81" t="s">
         <v>136</v>
@@ -5890,7 +5875,7 @@
       <c r="I118" s="82"/>
       <c r="J118" s="83"/>
       <c r="K118" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L118" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5908,7 +5893,7 @@
         <v>72</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
@@ -5917,7 +5902,7 @@
       <c r="I119" s="7"/>
       <c r="J119" s="8"/>
       <c r="K119" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L119" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5935,7 +5920,7 @@
         <v>72</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
@@ -5944,7 +5929,7 @@
       <c r="I120" s="7"/>
       <c r="J120" s="8"/>
       <c r="K120" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L120" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5962,7 +5947,7 @@
         <v>72</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
@@ -5971,7 +5956,7 @@
       <c r="I121" s="7"/>
       <c r="J121" s="8"/>
       <c r="K121" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L121" s="9" t="str">
         <f t="shared" si="1"/>
@@ -5989,10 +5974,10 @@
         <v>73</v>
       </c>
       <c r="D122" s="60" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E122" s="58" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F122" s="58" t="s">
         <v>136</v>
@@ -6002,7 +5987,7 @@
       <c r="I122" s="61"/>
       <c r="J122" s="62"/>
       <c r="K122" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L122" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6020,14 +6005,14 @@
         <v>129</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
       <c r="H123" s="9"/>
       <c r="J123" s="37"/>
       <c r="K123" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L123" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6045,14 +6030,14 @@
         <v>74</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E124" s="7"/>
       <c r="F124" s="7"/>
       <c r="H124" s="38"/>
       <c r="I124" s="38"/>
       <c r="K124" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L124" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6070,7 +6055,7 @@
         <v>11</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
@@ -6079,7 +6064,7 @@
       <c r="I125" s="13"/>
       <c r="J125" s="4"/>
       <c r="K125" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L125" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6097,7 +6082,7 @@
         <v>76</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
@@ -6106,7 +6091,7 @@
       <c r="I126" s="13"/>
       <c r="J126" s="4"/>
       <c r="K126" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L126" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6124,7 +6109,7 @@
         <v>77</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
@@ -6133,7 +6118,7 @@
       <c r="I127" s="13"/>
       <c r="J127" s="4"/>
       <c r="K127" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L127" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6151,7 +6136,7 @@
         <v>178</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E128" s="6"/>
       <c r="F128" s="6"/>
@@ -6160,7 +6145,7 @@
       <c r="I128" s="32"/>
       <c r="J128" s="6"/>
       <c r="K128" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L128" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6178,7 +6163,7 @@
         <v>11</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
@@ -6187,7 +6172,7 @@
       <c r="I129" s="42"/>
       <c r="J129" s="34"/>
       <c r="K129" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L129" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6205,7 +6190,7 @@
         <v>127</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
@@ -6214,7 +6199,7 @@
       <c r="I130" s="42"/>
       <c r="J130" s="34"/>
       <c r="K130" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L130" s="9" t="str">
         <f t="shared" si="1"/>
@@ -6232,7 +6217,7 @@
         <v>80</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E131" s="12"/>
       <c r="F131" s="12"/>
@@ -6241,7 +6226,7 @@
       <c r="I131" s="42"/>
       <c r="J131" s="12"/>
       <c r="K131" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L131" s="9" t="str">
         <f t="shared" ref="L131:L194" si="2">IF(K131="Yellow", "50%", IF(K131="Green", "100%", IF(K131="Grey", "0%", IF(K131="White", "30%", IF(K131="Orange", "10%", "")))))</f>
@@ -6259,7 +6244,7 @@
         <v>81</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E132" s="4"/>
       <c r="F132" s="4" t="s">
@@ -6270,7 +6255,7 @@
       <c r="I132" s="43"/>
       <c r="J132" s="4"/>
       <c r="K132" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L132" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6285,10 +6270,10 @@
         <v>79</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
@@ -6297,7 +6282,7 @@
       <c r="I133" s="43"/>
       <c r="J133" s="4"/>
       <c r="K133" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L133" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6315,7 +6300,7 @@
         <v>179</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E134" s="4"/>
       <c r="F134" s="12"/>
@@ -6324,7 +6309,7 @@
       <c r="I134" s="42"/>
       <c r="J134" s="12"/>
       <c r="K134" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L134" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6342,7 +6327,7 @@
         <v>180</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E135" s="4"/>
       <c r="F135" s="4" t="s">
@@ -6353,7 +6338,7 @@
       <c r="I135" s="42"/>
       <c r="J135" s="12"/>
       <c r="K135" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L135" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6371,7 +6356,7 @@
         <v>180</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E136" s="4"/>
       <c r="F136" s="4" t="s">
@@ -6382,7 +6367,7 @@
       <c r="I136" s="42"/>
       <c r="J136" s="12"/>
       <c r="K136" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L136" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6400,7 +6385,7 @@
         <v>82</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
@@ -6409,7 +6394,7 @@
       <c r="I137" s="42"/>
       <c r="J137" s="12"/>
       <c r="K137" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L137" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6427,7 +6412,7 @@
         <v>181</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
@@ -6436,7 +6421,7 @@
       <c r="I138" s="42"/>
       <c r="J138" s="12"/>
       <c r="K138" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L138" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6454,7 +6439,7 @@
         <v>83</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
@@ -6463,7 +6448,7 @@
       <c r="I139" s="42"/>
       <c r="J139" s="12"/>
       <c r="K139" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L139" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6481,7 +6466,7 @@
         <v>182</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
@@ -6490,7 +6475,7 @@
       <c r="I140" s="42"/>
       <c r="J140" s="12"/>
       <c r="K140" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L140" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6508,7 +6493,7 @@
         <v>183</v>
       </c>
       <c r="D141" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
@@ -6517,7 +6502,7 @@
       <c r="I141" s="42"/>
       <c r="J141" s="12"/>
       <c r="K141" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L141" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6535,7 +6520,7 @@
         <v>84</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E142" s="44"/>
       <c r="F142" s="4" t="s">
@@ -6546,7 +6531,7 @@
       <c r="I142" s="42"/>
       <c r="J142" s="12"/>
       <c r="K142" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L142" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6564,7 +6549,7 @@
         <v>85</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E143" s="18"/>
       <c r="F143" s="4"/>
@@ -6573,7 +6558,7 @@
       <c r="I143" s="2"/>
       <c r="J143" s="2"/>
       <c r="K143" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L143" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6591,7 +6576,7 @@
         <v>11</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E144" s="15"/>
       <c r="F144" s="4"/>
@@ -6600,7 +6585,7 @@
       <c r="I144" s="7"/>
       <c r="J144" s="8"/>
       <c r="K144" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L144" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6618,7 +6603,7 @@
         <v>184</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E145" s="12"/>
       <c r="F145" s="12" t="s">
@@ -6629,7 +6614,7 @@
       <c r="I145" s="7"/>
       <c r="J145" s="8"/>
       <c r="K145" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L145" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6647,7 +6632,7 @@
         <v>185</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E146" s="44"/>
       <c r="F146" s="4" t="s">
@@ -6658,7 +6643,7 @@
       <c r="I146" s="7"/>
       <c r="J146" s="8"/>
       <c r="K146" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L146" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6676,7 +6661,7 @@
         <v>185</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E147" s="44"/>
       <c r="F147" s="4" t="s">
@@ -6687,7 +6672,7 @@
       <c r="I147" s="7"/>
       <c r="J147" s="8"/>
       <c r="K147" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L147" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6705,7 +6690,7 @@
         <v>11</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E148" s="12"/>
       <c r="F148" s="12"/>
@@ -6714,7 +6699,7 @@
       <c r="I148" s="13"/>
       <c r="J148" s="8"/>
       <c r="K148" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L148" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6730,7 +6715,7 @@
         <v>88</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
@@ -6739,7 +6724,7 @@
       <c r="I149" s="8"/>
       <c r="J149" s="8"/>
       <c r="K149" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L149" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6757,7 +6742,7 @@
         <v>11</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E150" s="6"/>
       <c r="F150" s="6"/>
@@ -6766,7 +6751,7 @@
       <c r="I150" s="2"/>
       <c r="J150" s="8"/>
       <c r="K150" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L150" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6784,7 +6769,7 @@
         <v>187</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E151" s="6"/>
       <c r="F151" s="6"/>
@@ -6793,7 +6778,7 @@
       <c r="I151" s="7"/>
       <c r="J151" s="8"/>
       <c r="K151" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L151" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6811,7 +6796,7 @@
         <v>188</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E152" s="6"/>
       <c r="F152" s="4"/>
@@ -6820,7 +6805,7 @@
       <c r="I152" s="7"/>
       <c r="J152" s="8"/>
       <c r="K152" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L152" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6838,7 +6823,7 @@
         <v>189</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E153" s="6"/>
       <c r="F153" s="4"/>
@@ -6847,7 +6832,7 @@
       <c r="I153" s="8"/>
       <c r="J153" s="8"/>
       <c r="K153" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L153" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6865,7 +6850,7 @@
         <v>190</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E154" s="6"/>
       <c r="F154" s="4"/>
@@ -6874,7 +6859,7 @@
       <c r="I154" s="8"/>
       <c r="J154" s="8"/>
       <c r="K154" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L154" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6892,7 +6877,7 @@
         <v>190</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E155" s="6"/>
       <c r="F155" s="4"/>
@@ -6901,7 +6886,7 @@
       <c r="I155" s="8"/>
       <c r="J155" s="8"/>
       <c r="K155" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L155" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6919,7 +6904,7 @@
         <v>190</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E156" s="6"/>
       <c r="F156" s="4"/>
@@ -6928,7 +6913,7 @@
       <c r="I156" s="8"/>
       <c r="J156" s="8"/>
       <c r="K156" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L156" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6946,7 +6931,7 @@
         <v>126</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E157" s="6"/>
       <c r="F157" s="4"/>
@@ -6955,7 +6940,7 @@
       <c r="I157" s="8"/>
       <c r="J157" s="8"/>
       <c r="K157" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L157" s="9" t="str">
         <f t="shared" si="2"/>
@@ -6973,7 +6958,7 @@
         <v>126</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E158" s="6"/>
       <c r="F158" s="4"/>
@@ -6982,7 +6967,7 @@
       <c r="I158" s="8"/>
       <c r="J158" s="8"/>
       <c r="K158" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L158" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7000,7 +6985,7 @@
         <v>191</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E159" s="6"/>
       <c r="F159" s="4"/>
@@ -7009,7 +6994,7 @@
       <c r="I159" s="8"/>
       <c r="J159" s="8"/>
       <c r="K159" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L159" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7027,10 +7012,10 @@
         <v>192</v>
       </c>
       <c r="D160" s="97" t="s">
-        <v>282</v>
-      </c>
-      <c r="E160" s="100" t="s">
-        <v>256</v>
+        <v>280</v>
+      </c>
+      <c r="E160" s="98" t="s">
+        <v>255</v>
       </c>
       <c r="F160" s="88" t="s">
         <v>201</v>
@@ -7040,7 +7025,7 @@
       <c r="I160" s="92"/>
       <c r="J160" s="92"/>
       <c r="K160" s="93" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="L160" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7059,7 +7044,7 @@
         <v>131</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E161" s="6"/>
       <c r="F161" s="7" t="s">
@@ -7070,7 +7055,7 @@
       <c r="I161" s="8"/>
       <c r="J161" s="8"/>
       <c r="K161" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L161" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7088,7 +7073,7 @@
         <v>193</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E162" s="6"/>
       <c r="F162" s="7"/>
@@ -7097,7 +7082,7 @@
       <c r="I162" s="8"/>
       <c r="J162" s="8"/>
       <c r="K162" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L162" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7115,7 +7100,7 @@
         <v>194</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E163" s="6"/>
       <c r="F163" s="7"/>
@@ -7124,7 +7109,7 @@
       <c r="I163" s="8"/>
       <c r="J163" s="8"/>
       <c r="K163" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L163" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7142,7 +7127,7 @@
         <v>11</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E164" s="6"/>
       <c r="F164" s="7"/>
@@ -7151,7 +7136,7 @@
       <c r="I164" s="8"/>
       <c r="J164" s="8"/>
       <c r="K164" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L164" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7169,7 +7154,7 @@
         <v>195</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E165" s="6"/>
       <c r="F165" s="7"/>
@@ -7178,7 +7163,7 @@
       <c r="I165" s="8"/>
       <c r="J165" s="8"/>
       <c r="K165" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L165" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7196,7 +7181,7 @@
         <v>91</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E166" s="4"/>
       <c r="F166" s="4"/>
@@ -7205,7 +7190,7 @@
       <c r="I166" s="7"/>
       <c r="J166" s="8"/>
       <c r="K166" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L166" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7223,10 +7208,10 @@
         <v>92</v>
       </c>
       <c r="D167" s="81" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E167" s="81" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F167" s="81" t="s">
         <v>135</v>
@@ -7236,7 +7221,7 @@
       <c r="I167" s="83"/>
       <c r="J167" s="83"/>
       <c r="K167" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L167" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7255,7 +7240,7 @@
         <v>11</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E168" s="4"/>
       <c r="F168" s="4" t="s">
@@ -7266,7 +7251,7 @@
       <c r="I168" s="13"/>
       <c r="J168" s="8"/>
       <c r="K168" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L168" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7284,7 +7269,7 @@
         <v>11</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E169" s="4"/>
       <c r="F169" s="4" t="s">
@@ -7295,7 +7280,7 @@
       <c r="I169" s="13"/>
       <c r="J169" s="8"/>
       <c r="K169" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L169" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7313,7 +7298,7 @@
         <v>11</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E170" s="4"/>
       <c r="F170" s="4" t="s">
@@ -7324,7 +7309,7 @@
       <c r="I170" s="13"/>
       <c r="J170" s="8"/>
       <c r="K170" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L170" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7342,7 +7327,7 @@
         <v>11</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E171" s="4"/>
       <c r="F171" s="4" t="s">
@@ -7353,7 +7338,7 @@
       <c r="I171" s="13"/>
       <c r="J171" s="8"/>
       <c r="K171" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L171" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7371,12 +7356,12 @@
         <v>197</v>
       </c>
       <c r="D172" s="81" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E172" s="81" t="s">
-        <v>255</v>
-      </c>
-      <c r="F172" s="109" t="s">
+        <v>254</v>
+      </c>
+      <c r="F172" s="107" t="s">
         <v>214</v>
       </c>
       <c r="G172" s="82"/>
@@ -7384,7 +7369,7 @@
       <c r="I172" s="96"/>
       <c r="J172" s="83"/>
       <c r="K172" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L172" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7403,10 +7388,10 @@
         <v>196</v>
       </c>
       <c r="D173" s="88" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E173" s="88" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F173" s="89" t="s">
         <v>214</v>
@@ -7416,7 +7401,7 @@
       <c r="I173" s="91"/>
       <c r="J173" s="92"/>
       <c r="K173" s="93" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="L173" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7435,7 +7420,7 @@
         <v>198</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E174" s="4"/>
       <c r="F174" s="4"/>
@@ -7444,7 +7429,7 @@
       <c r="I174" s="13"/>
       <c r="J174" s="8"/>
       <c r="K174" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L174" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7462,7 +7447,7 @@
         <v>198</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E175" s="4"/>
       <c r="F175" s="4"/>
@@ -7471,7 +7456,7 @@
       <c r="I175" s="13"/>
       <c r="J175" s="8"/>
       <c r="K175" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L175" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7489,7 +7474,7 @@
         <v>198</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E176" s="4"/>
       <c r="F176" s="4"/>
@@ -7498,7 +7483,7 @@
       <c r="I176" s="13"/>
       <c r="J176" s="8"/>
       <c r="K176" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L176" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7516,7 +7501,7 @@
         <v>198</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E177" s="4"/>
       <c r="F177" s="4"/>
@@ -7525,7 +7510,7 @@
       <c r="I177" s="13"/>
       <c r="J177" s="8"/>
       <c r="K177" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L177" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7543,7 +7528,7 @@
         <v>94</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E178" s="4"/>
       <c r="F178" s="4"/>
@@ -7552,7 +7537,7 @@
       <c r="I178" s="13"/>
       <c r="J178" s="8"/>
       <c r="K178" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L178" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7570,7 +7555,7 @@
         <v>94</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E179" s="4"/>
       <c r="F179" s="4"/>
@@ -7579,7 +7564,7 @@
       <c r="I179" s="13"/>
       <c r="J179" s="8"/>
       <c r="K179" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L179" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7597,7 +7582,7 @@
         <v>94</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E180" s="4"/>
       <c r="F180" s="4"/>
@@ -7606,7 +7591,7 @@
       <c r="I180" s="13"/>
       <c r="J180" s="8"/>
       <c r="K180" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L180" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7624,7 +7609,7 @@
         <v>94</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E181" s="4"/>
       <c r="F181" s="4"/>
@@ -7633,7 +7618,7 @@
       <c r="I181" s="13"/>
       <c r="J181" s="8"/>
       <c r="K181" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L181" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7651,7 +7636,7 @@
         <v>199</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E182" s="4"/>
       <c r="F182" s="4"/>
@@ -7660,7 +7645,7 @@
       <c r="I182" s="13"/>
       <c r="J182" s="8"/>
       <c r="K182" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L182" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7678,10 +7663,10 @@
         <v>200</v>
       </c>
       <c r="D183" s="58" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E183" s="63" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F183" s="58" t="s">
         <v>218</v>
@@ -7691,7 +7676,7 @@
       <c r="I183" s="75"/>
       <c r="J183" s="62"/>
       <c r="K183" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L183" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7707,10 +7692,10 @@
         <v>96</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E184" s="4"/>
       <c r="F184" s="4"/>
@@ -7719,7 +7704,7 @@
       <c r="I184" s="2"/>
       <c r="J184" s="2"/>
       <c r="K184" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L184" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7734,10 +7719,10 @@
         <v>96</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E185" s="4"/>
       <c r="F185" s="4"/>
@@ -7746,7 +7731,7 @@
       <c r="I185" s="2"/>
       <c r="J185" s="2"/>
       <c r="K185" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L185" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7761,10 +7746,10 @@
         <v>97</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E186" s="4"/>
       <c r="F186" s="4"/>
@@ -7773,7 +7758,7 @@
       <c r="I186" s="26"/>
       <c r="J186" s="18"/>
       <c r="K186" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L186" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7788,10 +7773,10 @@
         <v>97</v>
       </c>
       <c r="C187" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D187" s="4" t="s">
         <v>279</v>
-      </c>
-      <c r="D187" s="4" t="s">
-        <v>281</v>
       </c>
       <c r="E187" s="4"/>
       <c r="F187" s="4"/>
@@ -7800,7 +7785,7 @@
       <c r="I187" s="26"/>
       <c r="J187" s="18"/>
       <c r="K187" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L187" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7815,10 +7800,10 @@
         <v>97</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E188" s="4"/>
       <c r="F188" s="4"/>
@@ -7827,7 +7812,7 @@
       <c r="I188" s="26"/>
       <c r="J188" s="18"/>
       <c r="K188" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L188" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7842,10 +7827,10 @@
         <v>97</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E189" s="4"/>
       <c r="F189" s="4"/>
@@ -7854,7 +7839,7 @@
       <c r="I189" s="26"/>
       <c r="J189" s="18"/>
       <c r="K189" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L189" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7869,10 +7854,10 @@
         <v>98</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E190" s="4"/>
       <c r="F190" s="4"/>
@@ -7881,7 +7866,7 @@
       <c r="I190" s="2"/>
       <c r="J190" s="4"/>
       <c r="K190" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L190" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7896,10 +7881,10 @@
         <v>99</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E191" s="4"/>
       <c r="F191" s="4"/>
@@ -7908,7 +7893,7 @@
       <c r="I191" s="7"/>
       <c r="J191" s="4"/>
       <c r="K191" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L191" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7923,10 +7908,10 @@
         <v>101</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E192" s="4"/>
       <c r="F192" s="4"/>
@@ -7935,7 +7920,7 @@
       <c r="I192" s="7"/>
       <c r="J192" s="4"/>
       <c r="K192" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L192" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7950,10 +7935,10 @@
         <v>102</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E193" s="4"/>
       <c r="F193" s="4"/>
@@ -7962,7 +7947,7 @@
       <c r="I193" s="8"/>
       <c r="J193" s="4"/>
       <c r="K193" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L193" s="9" t="str">
         <f t="shared" si="2"/>
@@ -7980,7 +7965,7 @@
         <v>87</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E194" s="6"/>
       <c r="F194" s="4"/>
@@ -7989,7 +7974,7 @@
       <c r="I194" s="8"/>
       <c r="J194" s="8"/>
       <c r="K194" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L194" s="9" t="str">
         <f t="shared" si="2"/>
@@ -8004,10 +7989,10 @@
         <v>128</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D195" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E195" s="6"/>
       <c r="F195" s="6"/>
@@ -8016,10 +8001,10 @@
       <c r="I195" s="8"/>
       <c r="J195" s="8"/>
       <c r="K195" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L195" s="9" t="str">
-        <f t="shared" ref="L195:L231" si="3">IF(K195="Yellow", "50%", IF(K195="Green", "100%", IF(K195="Grey", "0%", IF(K195="White", "30%", IF(K195="Orange", "10%", "")))))</f>
+        <f t="shared" ref="L195:L228" si="3">IF(K195="Yellow", "50%", IF(K195="Green", "100%", IF(K195="Grey", "0%", IF(K195="White", "30%", IF(K195="Orange", "10%", "")))))</f>
         <v>30%</v>
       </c>
     </row>
@@ -8031,10 +8016,10 @@
         <v>207</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E196" s="6"/>
       <c r="F196" s="6"/>
@@ -8043,7 +8028,7 @@
       <c r="I196" s="8"/>
       <c r="J196" s="8"/>
       <c r="K196" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L196" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8058,10 +8043,10 @@
         <v>104</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E197" s="6"/>
       <c r="F197" s="6"/>
@@ -8070,7 +8055,7 @@
       <c r="I197" s="8"/>
       <c r="J197" s="8"/>
       <c r="K197" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L197" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8085,10 +8070,10 @@
         <v>105</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D198" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E198" s="6"/>
       <c r="F198" s="6"/>
@@ -8097,7 +8082,7 @@
       <c r="I198" s="8"/>
       <c r="J198" s="8"/>
       <c r="K198" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L198" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8112,10 +8097,10 @@
         <v>106</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E199" s="6"/>
       <c r="F199" s="6"/>
@@ -8124,7 +8109,7 @@
       <c r="I199" s="8"/>
       <c r="J199" s="8"/>
       <c r="K199" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L199" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8139,10 +8124,10 @@
         <v>107</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E200" s="6"/>
       <c r="F200" s="6"/>
@@ -8151,7 +8136,7 @@
       <c r="I200" s="8"/>
       <c r="J200" s="4"/>
       <c r="K200" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L200" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8166,10 +8151,10 @@
         <v>108</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E201" s="6"/>
       <c r="F201" s="6"/>
@@ -8178,7 +8163,7 @@
       <c r="I201" s="8"/>
       <c r="J201" s="4"/>
       <c r="K201" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L201" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8193,10 +8178,10 @@
         <v>109</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E202" s="6"/>
       <c r="F202" s="6"/>
@@ -8205,7 +8190,7 @@
       <c r="I202" s="13"/>
       <c r="J202" s="4"/>
       <c r="K202" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L202" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8223,7 +8208,7 @@
         <v>87</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E203" s="15"/>
       <c r="F203" s="4"/>
@@ -8232,7 +8217,7 @@
       <c r="I203" s="7"/>
       <c r="J203" s="4"/>
       <c r="K203" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L203" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8248,10 +8233,10 @@
         <v>124</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E204" s="4"/>
       <c r="F204" s="4"/>
@@ -8260,7 +8245,7 @@
       <c r="I204" s="7"/>
       <c r="J204" s="4"/>
       <c r="K204" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L204" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8275,10 +8260,10 @@
         <v>123</v>
       </c>
       <c r="C205" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E205" s="4"/>
       <c r="F205" s="4"/>
@@ -8287,7 +8272,7 @@
       <c r="I205" s="7"/>
       <c r="J205" s="4"/>
       <c r="K205" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L205" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8302,10 +8287,10 @@
         <v>111</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E206" s="4"/>
       <c r="F206" s="4"/>
@@ -8314,7 +8299,7 @@
       <c r="I206" s="8"/>
       <c r="J206" s="8"/>
       <c r="K206" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L206" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8332,7 +8317,7 @@
         <v>87</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E207" s="6"/>
       <c r="F207" s="4"/>
@@ -8341,7 +8326,7 @@
       <c r="I207" s="8"/>
       <c r="J207" s="8"/>
       <c r="K207" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L207" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8359,10 +8344,10 @@
         <v>87</v>
       </c>
       <c r="D208" s="76" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E208" s="60" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F208" s="65"/>
       <c r="G208" s="75"/>
@@ -8370,7 +8355,7 @@
       <c r="I208" s="62"/>
       <c r="J208" s="62"/>
       <c r="K208" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L208" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8389,10 +8374,10 @@
         <v>87</v>
       </c>
       <c r="D209" s="76" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E209" s="60" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F209" s="65"/>
       <c r="G209" s="75"/>
@@ -8400,7 +8385,7 @@
       <c r="I209" s="62"/>
       <c r="J209" s="62"/>
       <c r="K209" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L209" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8419,10 +8404,10 @@
         <v>87</v>
       </c>
       <c r="D210" s="76" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E210" s="60" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F210" s="65"/>
       <c r="G210" s="75"/>
@@ -8430,7 +8415,7 @@
       <c r="I210" s="62"/>
       <c r="J210" s="62"/>
       <c r="K210" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L210" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8449,10 +8434,10 @@
         <v>87</v>
       </c>
       <c r="D211" s="76" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E211" s="60" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F211" s="65"/>
       <c r="G211" s="75"/>
@@ -8460,7 +8445,7 @@
       <c r="I211" s="62"/>
       <c r="J211" s="62"/>
       <c r="K211" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L211" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8474,10 +8459,10 @@
       </c>
       <c r="B212" s="66"/>
       <c r="C212" s="77" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D212" s="66" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E212" s="66" t="s">
         <v>208</v>
@@ -8488,7 +8473,7 @@
       <c r="I212" s="62"/>
       <c r="J212" s="62"/>
       <c r="K212" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L212" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8502,10 +8487,10 @@
       </c>
       <c r="B213" s="66"/>
       <c r="C213" s="77" t="s">
+        <v>277</v>
+      </c>
+      <c r="D213" s="66" t="s">
         <v>279</v>
-      </c>
-      <c r="D213" s="66" t="s">
-        <v>281</v>
       </c>
       <c r="E213" s="66" t="s">
         <v>208</v>
@@ -8516,7 +8501,7 @@
       <c r="I213" s="62"/>
       <c r="J213" s="62"/>
       <c r="K213" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L213" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8530,10 +8515,10 @@
       </c>
       <c r="B214" s="66"/>
       <c r="C214" s="77" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D214" s="66" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E214" s="66" t="s">
         <v>208</v>
@@ -8544,7 +8529,7 @@
       <c r="I214" s="62"/>
       <c r="J214" s="62"/>
       <c r="K214" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L214" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8558,10 +8543,10 @@
       </c>
       <c r="B215" s="66"/>
       <c r="C215" s="77" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D215" s="66" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E215" s="66" t="s">
         <v>208</v>
@@ -8572,7 +8557,7 @@
       <c r="I215" s="62"/>
       <c r="J215" s="62"/>
       <c r="K215" s="63" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L215" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8591,7 +8576,7 @@
         <v>210</v>
       </c>
       <c r="D216" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E216" s="39" t="s">
         <v>211</v>
@@ -8602,7 +8587,7 @@
       <c r="I216" s="8"/>
       <c r="J216" s="8"/>
       <c r="K216" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L216" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8620,7 +8605,7 @@
         <v>210</v>
       </c>
       <c r="D217" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E217" s="39" t="s">
         <v>211</v>
@@ -8631,7 +8616,7 @@
       <c r="I217" s="8"/>
       <c r="J217" s="8"/>
       <c r="K217" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L217" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8649,7 +8634,7 @@
         <v>210</v>
       </c>
       <c r="D218" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E218" s="39" t="s">
         <v>211</v>
@@ -8660,7 +8645,7 @@
       <c r="I218" s="8"/>
       <c r="J218" s="8"/>
       <c r="K218" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L218" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8678,7 +8663,7 @@
         <v>210</v>
       </c>
       <c r="D219" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E219" s="39" t="s">
         <v>211</v>
@@ -8689,7 +8674,7 @@
       <c r="I219" s="8"/>
       <c r="J219" s="8"/>
       <c r="K219" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L219" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8704,10 +8689,10 @@
         <v>114</v>
       </c>
       <c r="C220" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E220" s="4"/>
       <c r="F220" s="4"/>
@@ -8716,7 +8701,7 @@
       <c r="I220" s="8"/>
       <c r="J220" s="8"/>
       <c r="K220" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L220" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8731,10 +8716,10 @@
         <v>115</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E221" s="17"/>
       <c r="F221" s="4"/>
@@ -8743,57 +8728,58 @@
       <c r="I221" s="8"/>
       <c r="J221" s="8"/>
       <c r="K221" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L221" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="222" spans="1:13" ht="13" x14ac:dyDescent="0.35">
-      <c r="A222" s="10" t="s">
+    <row r="222" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="A222" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="B222" s="4" t="s">
+      <c r="B222" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C222" s="4" t="s">
+      <c r="C222" s="82" t="s">
+        <v>244</v>
+      </c>
+      <c r="D222" s="82" t="s">
         <v>279</v>
       </c>
-      <c r="D222" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="E222" s="98" t="s">
-        <v>245</v>
-      </c>
-      <c r="F222" s="4"/>
-      <c r="G222" s="13"/>
-      <c r="H222" s="8"/>
-      <c r="I222" s="8"/>
-      <c r="J222" s="8"/>
-      <c r="K222" s="9" t="s">
-        <v>271</v>
+      <c r="E222" s="81" t="s">
+        <v>264</v>
+      </c>
+      <c r="F222" s="82"/>
+      <c r="G222" s="82"/>
+      <c r="H222" s="81"/>
+      <c r="I222" s="82"/>
+      <c r="J222" s="81"/>
+      <c r="K222" s="84" t="s">
+        <v>270</v>
       </c>
       <c r="L222" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>30%</v>
-      </c>
-    </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A223" s="10" t="s">
+        <v>100%</v>
+      </c>
+      <c r="M222" s="84"/>
+    </row>
+    <row r="223" spans="1:13" ht="39" x14ac:dyDescent="0.35">
+      <c r="A223" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B223" s="7" t="s">
         <v>115</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="D223" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="E223" s="4" t="s">
-        <v>244</v>
+        <v>275</v>
+      </c>
+      <c r="E223" s="81" t="s">
+        <v>266</v>
       </c>
       <c r="F223" s="7"/>
       <c r="G223" s="7"/>
@@ -8801,14 +8787,14 @@
       <c r="I223" s="7"/>
       <c r="J223" s="4"/>
       <c r="K223" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L223" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="224" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:13" ht="64.5" x14ac:dyDescent="0.35">
       <c r="A224" s="84" t="s">
         <v>100</v>
       </c>
@@ -8816,13 +8802,13 @@
         <v>115</v>
       </c>
       <c r="C224" s="82" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="D224" s="82" t="s">
         <v>281</v>
       </c>
       <c r="E224" s="81" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="F224" s="82"/>
       <c r="G224" s="82"/>
@@ -8830,7 +8816,7 @@
       <c r="I224" s="82"/>
       <c r="J224" s="81"/>
       <c r="K224" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L224" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8838,7 +8824,7 @@
       </c>
       <c r="M224" s="84"/>
     </row>
-    <row r="225" spans="1:13" ht="39" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A225" s="9" t="s">
         <v>100</v>
       </c>
@@ -8846,13 +8832,13 @@
         <v>115</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="D225" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="E225" s="81" t="s">
-        <v>268</v>
+        <v>280</v>
+      </c>
+      <c r="E225" s="44" t="s">
+        <v>258</v>
       </c>
       <c r="F225" s="7"/>
       <c r="G225" s="7"/>
@@ -8860,14 +8846,14 @@
       <c r="I225" s="7"/>
       <c r="J225" s="4"/>
       <c r="K225" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L225" s="9" t="str">
         <f t="shared" si="3"/>
         <v>30%</v>
       </c>
     </row>
-    <row r="226" spans="1:13" ht="51.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
       <c r="A226" s="84" t="s">
         <v>100</v>
       </c>
@@ -8875,13 +8861,13 @@
         <v>115</v>
       </c>
       <c r="C226" s="82" t="s">
+        <v>244</v>
+      </c>
+      <c r="D226" s="82" t="s">
         <v>279</v>
       </c>
-      <c r="D226" s="82" t="s">
-        <v>283</v>
-      </c>
       <c r="E226" s="81" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="F226" s="82"/>
       <c r="G226" s="82"/>
@@ -8889,7 +8875,7 @@
       <c r="I226" s="82"/>
       <c r="J226" s="81"/>
       <c r="K226" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L226" s="9" t="str">
         <f t="shared" si="3"/>
@@ -8897,36 +8883,37 @@
       </c>
       <c r="M226" s="84"/>
     </row>
-    <row r="227" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A227" s="9" t="s">
+    <row r="227" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A227" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="B227" s="7" t="s">
+      <c r="B227" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C227" s="7" t="s">
+      <c r="C227" s="82" t="s">
+        <v>253</v>
+      </c>
+      <c r="D227" s="82" t="s">
         <v>279</v>
       </c>
-      <c r="D227" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="E227" s="44" t="s">
-        <v>260</v>
-      </c>
-      <c r="F227" s="7"/>
-      <c r="G227" s="7"/>
-      <c r="H227" s="4"/>
-      <c r="I227" s="7"/>
-      <c r="J227" s="4"/>
-      <c r="K227" s="9" t="s">
-        <v>271</v>
+      <c r="E227" s="82" t="s">
+        <v>265</v>
+      </c>
+      <c r="F227" s="82"/>
+      <c r="G227" s="82"/>
+      <c r="H227" s="81"/>
+      <c r="I227" s="82"/>
+      <c r="J227" s="81"/>
+      <c r="K227" s="84" t="s">
+        <v>270</v>
       </c>
       <c r="L227" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>30%</v>
-      </c>
-    </row>
-    <row r="228" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+        <v>100%</v>
+      </c>
+      <c r="M227" s="84"/>
+    </row>
+    <row r="228" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A228" s="84" t="s">
         <v>100</v>
       </c>
@@ -8934,12 +8921,12 @@
         <v>115</v>
       </c>
       <c r="C228" s="82" t="s">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="D228" s="82" t="s">
         <v>281</v>
       </c>
-      <c r="E228" s="81" t="s">
+      <c r="E228" s="82" t="s">
         <v>265</v>
       </c>
       <c r="F228" s="82"/>
@@ -8948,102 +8935,13 @@
       <c r="I228" s="82"/>
       <c r="J228" s="81"/>
       <c r="K228" s="84" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L228" s="9" t="str">
         <f t="shared" si="3"/>
         <v>100%</v>
       </c>
       <c r="M228" s="84"/>
-    </row>
-    <row r="229" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A229" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B229" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C229" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="D229" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="E229" s="99" t="s">
-        <v>254</v>
-      </c>
-      <c r="F229" s="7"/>
-      <c r="G229" s="7"/>
-      <c r="H229" s="4"/>
-      <c r="I229" s="7"/>
-      <c r="J229" s="4"/>
-      <c r="K229" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="L229" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>30%</v>
-      </c>
-    </row>
-    <row r="230" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A230" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="B230" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="C230" s="82" t="s">
-        <v>279</v>
-      </c>
-      <c r="D230" s="82" t="s">
-        <v>281</v>
-      </c>
-      <c r="E230" s="82" t="s">
-        <v>267</v>
-      </c>
-      <c r="F230" s="82"/>
-      <c r="G230" s="82"/>
-      <c r="H230" s="81"/>
-      <c r="I230" s="82"/>
-      <c r="J230" s="81"/>
-      <c r="K230" s="84" t="s">
-        <v>272</v>
-      </c>
-      <c r="L230" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>100%</v>
-      </c>
-      <c r="M230" s="84"/>
-    </row>
-    <row r="231" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
-      <c r="A231" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="B231" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="C231" s="82" t="s">
-        <v>279</v>
-      </c>
-      <c r="D231" s="82" t="s">
-        <v>283</v>
-      </c>
-      <c r="E231" s="82" t="s">
-        <v>267</v>
-      </c>
-      <c r="F231" s="82"/>
-      <c r="G231" s="82"/>
-      <c r="H231" s="81"/>
-      <c r="I231" s="82"/>
-      <c r="J231" s="81"/>
-      <c r="K231" s="84" t="s">
-        <v>272</v>
-      </c>
-      <c r="L231" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v>100%</v>
-      </c>
-      <c r="M231" s="84"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I71:I73">
@@ -9098,12 +8996,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
@@ -9134,12 +9032,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="109" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
     </row>
     <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
@@ -9418,12 +9316,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="56" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>